<commit_message>
config excel report and rename varible name
</commit_message>
<xml_diff>
--- a/public/templates/report_templateV2.xlsx
+++ b/public/templates/report_templateV2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcastillo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gpro1\MyFiles\QuisVar\quisvar_proyect_ft\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C486BD46-7045-48B3-8590-13D5FF7B9AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01464138-FCC9-4A14-BA0A-6E7CC6B6A9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="482" firstSheet="1" activeTab="1" xr2:uid="{F98A2DB2-54A5-485C-A701-CE43CF6B2BAF}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <definedName name="_Hlk78726999" localSheetId="1">'PERIDO 18'!#REF!</definedName>
     <definedName name="_Hlk87049115" localSheetId="1">'PERIDO 18'!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">LIQUIDACION!$A$1:$BD$173</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'PERIDO 18'!$A$1:$L$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'PERIDO 18'!$A$1:$K$36</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">LIQUIDACION!$1:$7</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'PERIDO 18'!$1:$26</definedName>
   </definedNames>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="370">
   <si>
     <t>ITEM</t>
   </si>
@@ -1645,9 +1645,6 @@
   </si>
   <si>
     <t>INFORME PARCIAL DE SERVICIOS PROFESIONALES Nº 004-2023-ASISTENTE DEL AREA DE INSTALACIONES SANITARIAS/V.A.T.M.</t>
-  </si>
-  <si>
-    <t>INFORME PARCIAL DE SERVICIOS PROFESIONALES PRESTADOS COMO COORDINADOR DEL AREA SANITARIAS DE PROYECTOS</t>
   </si>
   <si>
     <t xml:space="preserve">CC  COORDINADOR DE ESTRUCTURAS : </t>
@@ -3067,7 +3064,7 @@
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="344">
+  <cellXfs count="341">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3663,6 +3660,147 @@
     <xf numFmtId="0" fontId="38" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="9" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="9" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -3681,107 +3819,26 @@
     <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="2" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3789,6 +3846,72 @@
     <xf numFmtId="0" fontId="34" fillId="2" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="9" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="9" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="9" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3801,69 +3924,12 @@
     <xf numFmtId="0" fontId="23" fillId="9" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="9" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="9" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="9" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="9" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3879,60 +3945,6 @@
     <xf numFmtId="0" fontId="23" fillId="3" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3989,30 +4001,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="9" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="9" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -4375,174 +4363,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="261" t="s">
+      <c r="A1" s="255" t="s">
         <v>328</v>
       </c>
-      <c r="B1" s="260"/>
-      <c r="C1" s="260"/>
-      <c r="D1" s="260"/>
-      <c r="E1" s="260"/>
-      <c r="F1" s="260"/>
-      <c r="G1" s="260"/>
-      <c r="H1" s="260"/>
-      <c r="I1" s="260"/>
-      <c r="J1" s="260"/>
-      <c r="K1" s="260"/>
-      <c r="L1" s="260"/>
-      <c r="M1" s="260"/>
-      <c r="N1" s="260"/>
-      <c r="O1" s="259" t="s">
+      <c r="B1" s="254"/>
+      <c r="C1" s="254"/>
+      <c r="D1" s="254"/>
+      <c r="E1" s="254"/>
+      <c r="F1" s="254"/>
+      <c r="G1" s="254"/>
+      <c r="H1" s="254"/>
+      <c r="I1" s="254"/>
+      <c r="J1" s="254"/>
+      <c r="K1" s="254"/>
+      <c r="L1" s="254"/>
+      <c r="M1" s="254"/>
+      <c r="N1" s="254"/>
+      <c r="O1" s="253" t="s">
         <v>326</v>
       </c>
-      <c r="P1" s="259"/>
-      <c r="Q1" s="259"/>
-      <c r="R1" s="259"/>
-      <c r="S1" s="259"/>
-      <c r="T1" s="259"/>
-      <c r="U1" s="259"/>
-      <c r="V1" s="259"/>
-      <c r="W1" s="259"/>
-      <c r="X1" s="259"/>
-      <c r="Y1" s="259"/>
-      <c r="Z1" s="259"/>
-      <c r="AA1" s="259"/>
-      <c r="AB1" s="259"/>
-      <c r="AC1" s="259"/>
-      <c r="AD1" s="259"/>
-      <c r="AE1" s="259"/>
-      <c r="AF1" s="259"/>
-      <c r="AG1" s="259"/>
-      <c r="AH1" s="260" t="s">
+      <c r="P1" s="253"/>
+      <c r="Q1" s="253"/>
+      <c r="R1" s="253"/>
+      <c r="S1" s="253"/>
+      <c r="T1" s="253"/>
+      <c r="U1" s="253"/>
+      <c r="V1" s="253"/>
+      <c r="W1" s="253"/>
+      <c r="X1" s="253"/>
+      <c r="Y1" s="253"/>
+      <c r="Z1" s="253"/>
+      <c r="AA1" s="253"/>
+      <c r="AB1" s="253"/>
+      <c r="AC1" s="253"/>
+      <c r="AD1" s="253"/>
+      <c r="AE1" s="253"/>
+      <c r="AF1" s="253"/>
+      <c r="AG1" s="253"/>
+      <c r="AH1" s="254" t="s">
         <v>320</v>
       </c>
-      <c r="AI1" s="260"/>
-      <c r="AJ1" s="260"/>
-      <c r="AK1" s="260"/>
-      <c r="AL1" s="257" t="s">
+      <c r="AI1" s="254"/>
+      <c r="AJ1" s="254"/>
+      <c r="AK1" s="254"/>
+      <c r="AL1" s="251" t="s">
         <v>327</v>
       </c>
-      <c r="AM1" s="257"/>
-      <c r="AN1" s="257"/>
-      <c r="AO1" s="257"/>
-      <c r="AP1" s="257"/>
-      <c r="AQ1" s="257"/>
-      <c r="AR1" s="257"/>
-      <c r="AS1" s="257"/>
-      <c r="AT1" s="257"/>
-      <c r="AU1" s="257"/>
-      <c r="AV1" s="257"/>
-      <c r="AW1" s="257"/>
-      <c r="AX1" s="257"/>
-      <c r="AY1" s="257"/>
-      <c r="AZ1" s="257"/>
-      <c r="BA1" s="257"/>
-      <c r="BB1" s="257"/>
-      <c r="BC1" s="257"/>
-      <c r="BD1" s="258"/>
+      <c r="AM1" s="251"/>
+      <c r="AN1" s="251"/>
+      <c r="AO1" s="251"/>
+      <c r="AP1" s="251"/>
+      <c r="AQ1" s="251"/>
+      <c r="AR1" s="251"/>
+      <c r="AS1" s="251"/>
+      <c r="AT1" s="251"/>
+      <c r="AU1" s="251"/>
+      <c r="AV1" s="251"/>
+      <c r="AW1" s="251"/>
+      <c r="AX1" s="251"/>
+      <c r="AY1" s="251"/>
+      <c r="AZ1" s="251"/>
+      <c r="BA1" s="251"/>
+      <c r="BB1" s="251"/>
+      <c r="BC1" s="251"/>
+      <c r="BD1" s="252"/>
     </row>
     <row r="2" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="227" t="s">
+      <c r="A2" s="274" t="s">
         <v>294</v>
       </c>
-      <c r="B2" s="228"/>
+      <c r="B2" s="275"/>
       <c r="C2" s="141" t="s">
         <v>287</v>
       </c>
-      <c r="D2" s="231" t="s">
+      <c r="D2" s="278" t="s">
         <v>330</v>
       </c>
-      <c r="E2" s="231"/>
-      <c r="F2" s="263" t="s">
+      <c r="E2" s="278"/>
+      <c r="F2" s="243" t="s">
         <v>329</v>
       </c>
-      <c r="G2" s="263"/>
-      <c r="H2" s="263"/>
-      <c r="I2" s="263"/>
-      <c r="J2" s="263"/>
-      <c r="K2" s="263"/>
-      <c r="L2" s="263"/>
-      <c r="M2" s="263"/>
-      <c r="N2" s="263"/>
-      <c r="O2" s="263"/>
-      <c r="P2" s="263"/>
-      <c r="Q2" s="263"/>
-      <c r="R2" s="263"/>
-      <c r="S2" s="263"/>
-      <c r="T2" s="263"/>
-      <c r="U2" s="263"/>
-      <c r="V2" s="263"/>
-      <c r="W2" s="263"/>
-      <c r="X2" s="263"/>
-      <c r="Y2" s="263"/>
-      <c r="Z2" s="263"/>
-      <c r="AA2" s="263"/>
-      <c r="AB2" s="263"/>
-      <c r="AC2" s="263"/>
-      <c r="AD2" s="263"/>
-      <c r="AE2" s="263"/>
-      <c r="AF2" s="263"/>
-      <c r="AG2" s="263"/>
-      <c r="AH2" s="263"/>
-      <c r="AI2" s="263"/>
-      <c r="AJ2" s="263"/>
-      <c r="AK2" s="263"/>
-      <c r="AL2" s="263"/>
-      <c r="AM2" s="263"/>
-      <c r="AN2" s="263"/>
-      <c r="AO2" s="263"/>
-      <c r="AP2" s="263"/>
-      <c r="AQ2" s="263"/>
-      <c r="AR2" s="263"/>
-      <c r="AS2" s="263"/>
-      <c r="AT2" s="263"/>
-      <c r="AU2" s="263"/>
-      <c r="AV2" s="263"/>
-      <c r="AW2" s="263"/>
-      <c r="AX2" s="263"/>
-      <c r="AY2" s="263"/>
-      <c r="AZ2" s="263"/>
-      <c r="BA2" s="263"/>
-      <c r="BB2" s="263"/>
-      <c r="BC2" s="263"/>
-      <c r="BD2" s="264"/>
+      <c r="G2" s="243"/>
+      <c r="H2" s="243"/>
+      <c r="I2" s="243"/>
+      <c r="J2" s="243"/>
+      <c r="K2" s="243"/>
+      <c r="L2" s="243"/>
+      <c r="M2" s="243"/>
+      <c r="N2" s="243"/>
+      <c r="O2" s="243"/>
+      <c r="P2" s="243"/>
+      <c r="Q2" s="243"/>
+      <c r="R2" s="243"/>
+      <c r="S2" s="243"/>
+      <c r="T2" s="243"/>
+      <c r="U2" s="243"/>
+      <c r="V2" s="243"/>
+      <c r="W2" s="243"/>
+      <c r="X2" s="243"/>
+      <c r="Y2" s="243"/>
+      <c r="Z2" s="243"/>
+      <c r="AA2" s="243"/>
+      <c r="AB2" s="243"/>
+      <c r="AC2" s="243"/>
+      <c r="AD2" s="243"/>
+      <c r="AE2" s="243"/>
+      <c r="AF2" s="243"/>
+      <c r="AG2" s="243"/>
+      <c r="AH2" s="243"/>
+      <c r="AI2" s="243"/>
+      <c r="AJ2" s="243"/>
+      <c r="AK2" s="243"/>
+      <c r="AL2" s="243"/>
+      <c r="AM2" s="243"/>
+      <c r="AN2" s="243"/>
+      <c r="AO2" s="243"/>
+      <c r="AP2" s="243"/>
+      <c r="AQ2" s="243"/>
+      <c r="AR2" s="243"/>
+      <c r="AS2" s="243"/>
+      <c r="AT2" s="243"/>
+      <c r="AU2" s="243"/>
+      <c r="AV2" s="243"/>
+      <c r="AW2" s="243"/>
+      <c r="AX2" s="243"/>
+      <c r="AY2" s="243"/>
+      <c r="AZ2" s="243"/>
+      <c r="BA2" s="243"/>
+      <c r="BB2" s="243"/>
+      <c r="BC2" s="243"/>
+      <c r="BD2" s="244"/>
     </row>
     <row r="3" spans="1:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="227" t="s">
+      <c r="A3" s="274" t="s">
         <v>295</v>
       </c>
-      <c r="B3" s="228"/>
+      <c r="B3" s="275"/>
       <c r="C3" s="141" t="s">
         <v>286</v>
       </c>
-      <c r="D3" s="256" t="s">
+      <c r="D3" s="257" t="s">
         <v>331</v>
       </c>
-      <c r="E3" s="256"/>
+      <c r="E3" s="257"/>
       <c r="F3" s="145">
         <v>75263586</v>
       </c>
       <c r="G3" s="145"/>
       <c r="H3" s="145"/>
-      <c r="I3" s="256" t="s">
+      <c r="I3" s="257" t="s">
         <v>335</v>
       </c>
-      <c r="J3" s="256"/>
-      <c r="K3" s="256"/>
-      <c r="L3" s="256"/>
-      <c r="M3" s="256"/>
-      <c r="N3" s="256"/>
-      <c r="O3" s="256"/>
-      <c r="P3" s="256"/>
-      <c r="Q3" s="256"/>
-      <c r="R3" s="266" t="s">
+      <c r="J3" s="257"/>
+      <c r="K3" s="257"/>
+      <c r="L3" s="257"/>
+      <c r="M3" s="257"/>
+      <c r="N3" s="257"/>
+      <c r="O3" s="257"/>
+      <c r="P3" s="257"/>
+      <c r="Q3" s="257"/>
+      <c r="R3" s="246" t="s">
         <v>337</v>
       </c>
-      <c r="S3" s="266"/>
-      <c r="T3" s="266"/>
-      <c r="U3" s="266"/>
-      <c r="V3" s="266"/>
-      <c r="W3" s="266"/>
-      <c r="X3" s="266"/>
+      <c r="S3" s="246"/>
+      <c r="T3" s="246"/>
+      <c r="U3" s="246"/>
+      <c r="V3" s="246"/>
+      <c r="W3" s="246"/>
+      <c r="X3" s="246"/>
       <c r="Y3" s="143"/>
       <c r="Z3" s="143"/>
       <c r="AA3" s="143"/>
@@ -4577,42 +4565,42 @@
       <c r="BD3" s="139"/>
     </row>
     <row r="4" spans="1:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="227" t="s">
+      <c r="A4" s="274" t="s">
         <v>296</v>
       </c>
-      <c r="B4" s="228"/>
+      <c r="B4" s="275"/>
       <c r="C4" s="141" t="s">
         <v>287</v>
       </c>
-      <c r="D4" s="256" t="s">
+      <c r="D4" s="257" t="s">
         <v>332</v>
       </c>
-      <c r="E4" s="256"/>
+      <c r="E4" s="257"/>
       <c r="F4" s="145">
         <v>99826036</v>
       </c>
       <c r="G4" s="145"/>
       <c r="H4" s="145"/>
-      <c r="I4" s="256" t="s">
+      <c r="I4" s="257" t="s">
         <v>336</v>
       </c>
-      <c r="J4" s="256"/>
-      <c r="K4" s="256"/>
-      <c r="L4" s="256"/>
-      <c r="M4" s="256"/>
-      <c r="N4" s="256"/>
-      <c r="O4" s="256"/>
-      <c r="P4" s="256"/>
-      <c r="Q4" s="256"/>
-      <c r="R4" s="266" t="s">
+      <c r="J4" s="257"/>
+      <c r="K4" s="257"/>
+      <c r="L4" s="257"/>
+      <c r="M4" s="257"/>
+      <c r="N4" s="257"/>
+      <c r="O4" s="257"/>
+      <c r="P4" s="257"/>
+      <c r="Q4" s="257"/>
+      <c r="R4" s="246" t="s">
         <v>338</v>
       </c>
-      <c r="S4" s="266"/>
-      <c r="T4" s="266"/>
-      <c r="U4" s="266"/>
-      <c r="V4" s="266"/>
-      <c r="W4" s="266"/>
-      <c r="X4" s="266"/>
+      <c r="S4" s="246"/>
+      <c r="T4" s="246"/>
+      <c r="U4" s="246"/>
+      <c r="V4" s="246"/>
+      <c r="W4" s="246"/>
+      <c r="X4" s="246"/>
       <c r="Y4" s="143"/>
       <c r="Z4" s="143"/>
       <c r="AA4" s="143"/>
@@ -4647,35 +4635,35 @@
       <c r="BD4" s="139"/>
     </row>
     <row r="5" spans="1:56" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="229" t="s">
+      <c r="A5" s="276" t="s">
         <v>302</v>
       </c>
-      <c r="B5" s="230"/>
+      <c r="B5" s="277"/>
       <c r="C5" s="142" t="s">
         <v>288</v>
       </c>
-      <c r="D5" s="232" t="s">
+      <c r="D5" s="279" t="s">
         <v>333</v>
       </c>
-      <c r="E5" s="232"/>
-      <c r="F5" s="265" t="s">
+      <c r="E5" s="279"/>
+      <c r="F5" s="245" t="s">
         <v>334</v>
       </c>
-      <c r="G5" s="265"/>
-      <c r="H5" s="265"/>
-      <c r="I5" s="265"/>
-      <c r="J5" s="265"/>
-      <c r="K5" s="265"/>
-      <c r="L5" s="265"/>
-      <c r="M5" s="265"/>
-      <c r="N5" s="265"/>
-      <c r="O5" s="265"/>
-      <c r="P5" s="265"/>
-      <c r="Q5" s="265"/>
-      <c r="R5" s="265"/>
-      <c r="S5" s="265"/>
-      <c r="T5" s="265"/>
-      <c r="U5" s="265"/>
+      <c r="G5" s="245"/>
+      <c r="H5" s="245"/>
+      <c r="I5" s="245"/>
+      <c r="J5" s="245"/>
+      <c r="K5" s="245"/>
+      <c r="L5" s="245"/>
+      <c r="M5" s="245"/>
+      <c r="N5" s="245"/>
+      <c r="O5" s="245"/>
+      <c r="P5" s="245"/>
+      <c r="Q5" s="245"/>
+      <c r="R5" s="245"/>
+      <c r="S5" s="245"/>
+      <c r="T5" s="245"/>
+      <c r="U5" s="245"/>
       <c r="V5" s="144"/>
       <c r="W5" s="144"/>
       <c r="X5" s="144"/>
@@ -4713,101 +4701,101 @@
       <c r="BD5" s="140"/>
     </row>
     <row r="6" spans="1:56" s="80" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="236" t="s">
+      <c r="A6" s="266" t="s">
         <v>313</v>
       </c>
-      <c r="B6" s="238" t="s">
+      <c r="B6" s="268" t="s">
         <v>160</v>
       </c>
-      <c r="C6" s="238" t="s">
+      <c r="C6" s="268" t="s">
         <v>157</v>
       </c>
-      <c r="D6" s="238" t="s">
+      <c r="D6" s="268" t="s">
         <v>292</v>
       </c>
-      <c r="E6" s="245" t="s">
+      <c r="E6" s="272" t="s">
         <v>159</v>
       </c>
-      <c r="F6" s="246"/>
-      <c r="G6" s="243" t="s">
+      <c r="F6" s="273"/>
+      <c r="G6" s="270" t="s">
         <v>293</v>
       </c>
-      <c r="H6" s="233" t="s">
+      <c r="H6" s="248" t="s">
         <v>135</v>
       </c>
-      <c r="I6" s="234"/>
-      <c r="J6" s="234"/>
-      <c r="K6" s="234"/>
-      <c r="L6" s="234"/>
-      <c r="M6" s="234"/>
-      <c r="N6" s="235"/>
-      <c r="O6" s="233" t="s">
+      <c r="I6" s="249"/>
+      <c r="J6" s="249"/>
+      <c r="K6" s="249"/>
+      <c r="L6" s="249"/>
+      <c r="M6" s="249"/>
+      <c r="N6" s="250"/>
+      <c r="O6" s="248" t="s">
         <v>136</v>
       </c>
-      <c r="P6" s="234"/>
-      <c r="Q6" s="234"/>
-      <c r="R6" s="234"/>
-      <c r="S6" s="234"/>
-      <c r="T6" s="234"/>
-      <c r="U6" s="235"/>
-      <c r="V6" s="233" t="s">
+      <c r="P6" s="249"/>
+      <c r="Q6" s="249"/>
+      <c r="R6" s="249"/>
+      <c r="S6" s="249"/>
+      <c r="T6" s="249"/>
+      <c r="U6" s="250"/>
+      <c r="V6" s="248" t="s">
         <v>1</v>
       </c>
-      <c r="W6" s="234"/>
-      <c r="X6" s="234"/>
-      <c r="Y6" s="234"/>
-      <c r="Z6" s="234"/>
-      <c r="AA6" s="234"/>
-      <c r="AB6" s="235"/>
-      <c r="AC6" s="233" t="s">
+      <c r="W6" s="249"/>
+      <c r="X6" s="249"/>
+      <c r="Y6" s="249"/>
+      <c r="Z6" s="249"/>
+      <c r="AA6" s="249"/>
+      <c r="AB6" s="250"/>
+      <c r="AC6" s="248" t="s">
         <v>137</v>
       </c>
-      <c r="AD6" s="234"/>
-      <c r="AE6" s="234"/>
-      <c r="AF6" s="234"/>
-      <c r="AG6" s="234"/>
-      <c r="AH6" s="234"/>
-      <c r="AI6" s="235"/>
-      <c r="AJ6" s="233" t="s">
+      <c r="AD6" s="249"/>
+      <c r="AE6" s="249"/>
+      <c r="AF6" s="249"/>
+      <c r="AG6" s="249"/>
+      <c r="AH6" s="249"/>
+      <c r="AI6" s="250"/>
+      <c r="AJ6" s="248" t="s">
         <v>84</v>
       </c>
-      <c r="AK6" s="234"/>
-      <c r="AL6" s="234"/>
-      <c r="AM6" s="234"/>
-      <c r="AN6" s="234"/>
-      <c r="AO6" s="234"/>
-      <c r="AP6" s="235"/>
-      <c r="AQ6" s="233" t="s">
+      <c r="AK6" s="249"/>
+      <c r="AL6" s="249"/>
+      <c r="AM6" s="249"/>
+      <c r="AN6" s="249"/>
+      <c r="AO6" s="249"/>
+      <c r="AP6" s="250"/>
+      <c r="AQ6" s="248" t="s">
         <v>138</v>
       </c>
-      <c r="AR6" s="234"/>
-      <c r="AS6" s="234"/>
-      <c r="AT6" s="234"/>
-      <c r="AU6" s="234"/>
-      <c r="AV6" s="234"/>
-      <c r="AW6" s="235"/>
-      <c r="AX6" s="233" t="s">
+      <c r="AR6" s="249"/>
+      <c r="AS6" s="249"/>
+      <c r="AT6" s="249"/>
+      <c r="AU6" s="249"/>
+      <c r="AV6" s="249"/>
+      <c r="AW6" s="250"/>
+      <c r="AX6" s="248" t="s">
         <v>139</v>
       </c>
-      <c r="AY6" s="234"/>
-      <c r="AZ6" s="234"/>
-      <c r="BA6" s="234"/>
-      <c r="BB6" s="234"/>
-      <c r="BC6" s="234"/>
-      <c r="BD6" s="235"/>
+      <c r="AY6" s="249"/>
+      <c r="AZ6" s="249"/>
+      <c r="BA6" s="249"/>
+      <c r="BB6" s="249"/>
+      <c r="BC6" s="249"/>
+      <c r="BD6" s="250"/>
     </row>
     <row r="7" spans="1:56" s="80" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="237"/>
-      <c r="B7" s="239"/>
-      <c r="C7" s="239"/>
-      <c r="D7" s="239"/>
+      <c r="A7" s="267"/>
+      <c r="B7" s="269"/>
+      <c r="C7" s="269"/>
+      <c r="D7" s="269"/>
       <c r="E7" s="154" t="s">
         <v>158</v>
       </c>
       <c r="F7" s="154" t="s">
         <v>312</v>
       </c>
-      <c r="G7" s="244"/>
+      <c r="G7" s="271"/>
       <c r="H7" s="155" t="s">
         <v>297</v>
       </c>
@@ -5081,7 +5069,7 @@
       <c r="BD9" s="89"/>
     </row>
     <row r="10" spans="1:56" s="80" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="240" t="s">
+      <c r="A10" s="262" t="s">
         <v>314</v>
       </c>
       <c r="B10" s="135"/>
@@ -5149,7 +5137,7 @@
       <c r="BD10" s="89"/>
     </row>
     <row r="11" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="241"/>
+      <c r="A11" s="263"/>
       <c r="B11" s="135"/>
       <c r="C11" s="90" t="s">
         <v>291</v>
@@ -5215,7 +5203,7 @@
       <c r="BD11" s="89"/>
     </row>
     <row r="12" spans="1:56" s="80" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="242"/>
+      <c r="A12" s="265"/>
       <c r="B12" s="135"/>
       <c r="C12" s="90" t="s">
         <v>89</v>
@@ -5405,7 +5393,7 @@
       <c r="BD14" s="89"/>
     </row>
     <row r="15" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="240" t="s">
+      <c r="A15" s="262" t="s">
         <v>315</v>
       </c>
       <c r="B15" s="135"/>
@@ -5475,7 +5463,7 @@
       <c r="BD15" s="89"/>
     </row>
     <row r="16" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="241"/>
+      <c r="A16" s="263"/>
       <c r="B16" s="135"/>
       <c r="C16" s="95" t="s">
         <v>104</v>
@@ -5543,7 +5531,7 @@
       <c r="BD16" s="89"/>
     </row>
     <row r="17" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="241"/>
+      <c r="A17" s="263"/>
       <c r="B17" s="135"/>
       <c r="C17" s="95" t="s">
         <v>105</v>
@@ -5611,7 +5599,7 @@
       <c r="BD17" s="89"/>
     </row>
     <row r="18" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="241"/>
+      <c r="A18" s="263"/>
       <c r="B18" s="135"/>
       <c r="C18" s="95" t="s">
         <v>106</v>
@@ -5679,7 +5667,7 @@
       <c r="BD18" s="89"/>
     </row>
     <row r="19" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="241"/>
+      <c r="A19" s="263"/>
       <c r="B19" s="135"/>
       <c r="C19" s="95" t="s">
         <v>99</v>
@@ -5747,7 +5735,7 @@
       <c r="BD19" s="89"/>
     </row>
     <row r="20" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="241"/>
+      <c r="A20" s="263"/>
       <c r="B20" s="135"/>
       <c r="C20" s="95" t="s">
         <v>107</v>
@@ -5815,7 +5803,7 @@
       <c r="BD20" s="89"/>
     </row>
     <row r="21" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="241"/>
+      <c r="A21" s="263"/>
       <c r="B21" s="135"/>
       <c r="C21" s="95" t="s">
         <v>108</v>
@@ -5883,7 +5871,7 @@
       <c r="BD21" s="89"/>
     </row>
     <row r="22" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="241"/>
+      <c r="A22" s="263"/>
       <c r="B22" s="135"/>
       <c r="C22" s="95" t="s">
         <v>109</v>
@@ -5951,7 +5939,7 @@
       <c r="BD22" s="89"/>
     </row>
     <row r="23" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="241"/>
+      <c r="A23" s="263"/>
       <c r="B23" s="135"/>
       <c r="C23" s="95" t="s">
         <v>110</v>
@@ -6019,7 +6007,7 @@
       <c r="BD23" s="89"/>
     </row>
     <row r="24" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="241"/>
+      <c r="A24" s="263"/>
       <c r="B24" s="135"/>
       <c r="C24" s="95" t="s">
         <v>111</v>
@@ -6087,7 +6075,7 @@
       <c r="BD24" s="89"/>
     </row>
     <row r="25" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="241"/>
+      <c r="A25" s="263"/>
       <c r="B25" s="135"/>
       <c r="C25" s="95" t="s">
         <v>112</v>
@@ -6155,7 +6143,7 @@
       <c r="BD25" s="89"/>
     </row>
     <row r="26" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="241"/>
+      <c r="A26" s="263"/>
       <c r="B26" s="135"/>
       <c r="C26" s="95" t="s">
         <v>113</v>
@@ -6223,7 +6211,7 @@
       <c r="BD26" s="89"/>
     </row>
     <row r="27" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="241"/>
+      <c r="A27" s="263"/>
       <c r="B27" s="135"/>
       <c r="C27" s="95" t="s">
         <v>114</v>
@@ -6291,7 +6279,7 @@
       <c r="BD27" s="89"/>
     </row>
     <row r="28" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="241"/>
+      <c r="A28" s="263"/>
       <c r="B28" s="135"/>
       <c r="C28" s="95" t="s">
         <v>115</v>
@@ -6359,7 +6347,7 @@
       <c r="BD28" s="89"/>
     </row>
     <row r="29" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="241"/>
+      <c r="A29" s="263"/>
       <c r="B29" s="135"/>
       <c r="C29" s="95" t="s">
         <v>116</v>
@@ -6427,7 +6415,7 @@
       <c r="BD29" s="89"/>
     </row>
     <row r="30" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="242"/>
+      <c r="A30" s="265"/>
       <c r="B30" s="135"/>
       <c r="C30" s="95" t="s">
         <v>117</v>
@@ -6557,7 +6545,7 @@
       <c r="BD31" s="89"/>
     </row>
     <row r="32" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="240" t="s">
+      <c r="A32" s="262" t="s">
         <v>316</v>
       </c>
       <c r="B32" s="135"/>
@@ -6625,7 +6613,7 @@
       <c r="BD32" s="89"/>
     </row>
     <row r="33" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="241"/>
+      <c r="A33" s="263"/>
       <c r="B33" s="135"/>
       <c r="C33" s="95" t="s">
         <v>105</v>
@@ -6691,7 +6679,7 @@
       <c r="BD33" s="89"/>
     </row>
     <row r="34" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="241"/>
+      <c r="A34" s="263"/>
       <c r="B34" s="135"/>
       <c r="C34" s="95" t="s">
         <v>108</v>
@@ -6757,7 +6745,7 @@
       <c r="BD34" s="89"/>
     </row>
     <row r="35" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="242"/>
+      <c r="A35" s="265"/>
       <c r="B35" s="135"/>
       <c r="C35" s="95" t="s">
         <v>91</v>
@@ -6885,7 +6873,7 @@
       <c r="BD36" s="89"/>
     </row>
     <row r="37" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="240" t="s">
+      <c r="A37" s="262" t="s">
         <v>317</v>
       </c>
       <c r="B37" s="136" t="s">
@@ -6949,7 +6937,7 @@
       <c r="BD37" s="89"/>
     </row>
     <row r="38" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="241"/>
+      <c r="A38" s="263"/>
       <c r="B38" s="137" t="s">
         <v>164</v>
       </c>
@@ -7017,7 +7005,7 @@
       <c r="BD38" s="89"/>
     </row>
     <row r="39" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="241"/>
+      <c r="A39" s="263"/>
       <c r="B39" s="137" t="s">
         <v>165</v>
       </c>
@@ -7085,7 +7073,7 @@
       <c r="BD39" s="89"/>
     </row>
     <row r="40" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="241"/>
+      <c r="A40" s="263"/>
       <c r="B40" s="136" t="s">
         <v>225</v>
       </c>
@@ -7147,7 +7135,7 @@
       <c r="BD40" s="89"/>
     </row>
     <row r="41" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="241"/>
+      <c r="A41" s="263"/>
       <c r="B41" s="137" t="s">
         <v>226</v>
       </c>
@@ -7215,7 +7203,7 @@
       <c r="BD41" s="89"/>
     </row>
     <row r="42" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="241"/>
+      <c r="A42" s="263"/>
       <c r="B42" s="136" t="s">
         <v>227</v>
       </c>
@@ -7277,7 +7265,7 @@
       <c r="BD42" s="89"/>
     </row>
     <row r="43" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="241"/>
+      <c r="A43" s="263"/>
       <c r="B43" s="137" t="s">
         <v>228</v>
       </c>
@@ -7341,7 +7329,7 @@
       <c r="BD43" s="89"/>
     </row>
     <row r="44" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="241"/>
+      <c r="A44" s="263"/>
       <c r="B44" s="135"/>
       <c r="C44" s="90" t="s">
         <v>174</v>
@@ -7407,7 +7395,7 @@
       <c r="BD44" s="89"/>
     </row>
     <row r="45" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="241"/>
+      <c r="A45" s="263"/>
       <c r="B45" s="135"/>
       <c r="C45" s="90" t="s">
         <v>173</v>
@@ -7473,7 +7461,7 @@
       <c r="BD45" s="89"/>
     </row>
     <row r="46" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="241"/>
+      <c r="A46" s="263"/>
       <c r="B46" s="136" t="s">
         <v>229</v>
       </c>
@@ -7535,7 +7523,7 @@
       <c r="BD46" s="89"/>
     </row>
     <row r="47" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="241"/>
+      <c r="A47" s="263"/>
       <c r="B47" s="137" t="s">
         <v>230</v>
       </c>
@@ -7603,7 +7591,7 @@
       <c r="BD47" s="89"/>
     </row>
     <row r="48" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="241"/>
+      <c r="A48" s="263"/>
       <c r="B48" s="137" t="s">
         <v>231</v>
       </c>
@@ -7671,7 +7659,7 @@
       <c r="BD48" s="89"/>
     </row>
     <row r="49" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="241"/>
+      <c r="A49" s="263"/>
       <c r="B49" s="137" t="s">
         <v>232</v>
       </c>
@@ -7739,7 +7727,7 @@
       <c r="BD49" s="89"/>
     </row>
     <row r="50" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="241"/>
+      <c r="A50" s="263"/>
       <c r="B50" s="137" t="s">
         <v>233</v>
       </c>
@@ -7807,7 +7795,7 @@
       <c r="BD50" s="89"/>
     </row>
     <row r="51" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="241"/>
+      <c r="A51" s="263"/>
       <c r="B51" s="136" t="s">
         <v>234</v>
       </c>
@@ -7869,7 +7857,7 @@
       <c r="BD51" s="89"/>
     </row>
     <row r="52" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="241"/>
+      <c r="A52" s="263"/>
       <c r="B52" s="137" t="s">
         <v>235</v>
       </c>
@@ -7937,7 +7925,7 @@
       <c r="BD52" s="89"/>
     </row>
     <row r="53" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="241"/>
+      <c r="A53" s="263"/>
       <c r="B53" s="137" t="s">
         <v>236</v>
       </c>
@@ -8005,7 +7993,7 @@
       <c r="BD53" s="89"/>
     </row>
     <row r="54" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="241"/>
+      <c r="A54" s="263"/>
       <c r="B54" s="136" t="s">
         <v>237</v>
       </c>
@@ -8067,7 +8055,7 @@
       <c r="BD54" s="89"/>
     </row>
     <row r="55" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="241"/>
+      <c r="A55" s="263"/>
       <c r="B55" s="137" t="s">
         <v>238</v>
       </c>
@@ -8133,7 +8121,7 @@
       <c r="BD55" s="89"/>
     </row>
     <row r="56" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="241"/>
+      <c r="A56" s="263"/>
       <c r="B56" s="135"/>
       <c r="C56" s="90" t="s">
         <v>183</v>
@@ -8201,7 +8189,7 @@
       <c r="BD56" s="89"/>
     </row>
     <row r="57" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="241"/>
+      <c r="A57" s="263"/>
       <c r="B57" s="135"/>
       <c r="C57" s="90" t="s">
         <v>182</v>
@@ -8269,7 +8257,7 @@
       <c r="BD57" s="89"/>
     </row>
     <row r="58" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="241"/>
+      <c r="A58" s="263"/>
       <c r="B58" s="137" t="s">
         <v>239</v>
       </c>
@@ -8335,7 +8323,7 @@
       <c r="BD58" s="89"/>
     </row>
     <row r="59" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="241"/>
+      <c r="A59" s="263"/>
       <c r="B59" s="135"/>
       <c r="C59" s="90" t="s">
         <v>282</v>
@@ -8403,7 +8391,7 @@
       <c r="BD59" s="89"/>
     </row>
     <row r="60" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="241"/>
+      <c r="A60" s="263"/>
       <c r="B60" s="135"/>
       <c r="C60" s="90" t="s">
         <v>283</v>
@@ -8471,7 +8459,7 @@
       <c r="BD60" s="89"/>
     </row>
     <row r="61" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="241"/>
+      <c r="A61" s="263"/>
       <c r="B61" s="136" t="s">
         <v>240</v>
       </c>
@@ -8533,7 +8521,7 @@
       <c r="BD61" s="89"/>
     </row>
     <row r="62" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="241"/>
+      <c r="A62" s="263"/>
       <c r="B62" s="137" t="s">
         <v>241</v>
       </c>
@@ -8601,7 +8589,7 @@
       <c r="BD62" s="89"/>
     </row>
     <row r="63" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="241"/>
+      <c r="A63" s="263"/>
       <c r="B63" s="137" t="s">
         <v>242</v>
       </c>
@@ -8669,7 +8657,7 @@
       <c r="BD63" s="89"/>
     </row>
     <row r="64" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="241"/>
+      <c r="A64" s="263"/>
       <c r="B64" s="136" t="s">
         <v>243</v>
       </c>
@@ -8731,7 +8719,7 @@
       <c r="BD64" s="89"/>
     </row>
     <row r="65" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="241"/>
+      <c r="A65" s="263"/>
       <c r="B65" s="137" t="s">
         <v>244</v>
       </c>
@@ -8799,7 +8787,7 @@
       <c r="BD65" s="89"/>
     </row>
     <row r="66" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="241"/>
+      <c r="A66" s="263"/>
       <c r="B66" s="136" t="s">
         <v>247</v>
       </c>
@@ -8861,7 +8849,7 @@
       <c r="BD66" s="89"/>
     </row>
     <row r="67" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="241"/>
+      <c r="A67" s="263"/>
       <c r="B67" s="137" t="s">
         <v>248</v>
       </c>
@@ -8929,7 +8917,7 @@
       <c r="BD67" s="89"/>
     </row>
     <row r="68" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="241"/>
+      <c r="A68" s="263"/>
       <c r="B68" s="136" t="s">
         <v>251</v>
       </c>
@@ -8991,7 +8979,7 @@
       <c r="BD68" s="89"/>
     </row>
     <row r="69" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="241"/>
+      <c r="A69" s="263"/>
       <c r="B69" s="137" t="s">
         <v>252</v>
       </c>
@@ -9059,7 +9047,7 @@
       <c r="BD69" s="89"/>
     </row>
     <row r="70" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="241"/>
+      <c r="A70" s="263"/>
       <c r="B70" s="137" t="s">
         <v>253</v>
       </c>
@@ -9127,7 +9115,7 @@
       <c r="BD70" s="89"/>
     </row>
     <row r="71" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="241"/>
+      <c r="A71" s="263"/>
       <c r="B71" s="136" t="s">
         <v>254</v>
       </c>
@@ -9189,7 +9177,7 @@
       <c r="BD71" s="89"/>
     </row>
     <row r="72" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="241"/>
+      <c r="A72" s="263"/>
       <c r="B72" s="137" t="s">
         <v>255</v>
       </c>
@@ -9257,7 +9245,7 @@
       <c r="BD72" s="89"/>
     </row>
     <row r="73" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="241"/>
+      <c r="A73" s="263"/>
       <c r="B73" s="136" t="s">
         <v>256</v>
       </c>
@@ -9319,7 +9307,7 @@
       <c r="BD73" s="89"/>
     </row>
     <row r="74" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="242"/>
+      <c r="A74" s="265"/>
       <c r="B74" s="137" t="s">
         <v>257</v>
       </c>
@@ -9511,7 +9499,7 @@
       <c r="BD76" s="89"/>
     </row>
     <row r="77" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="240" t="s">
+      <c r="A77" s="262" t="s">
         <v>162</v>
       </c>
       <c r="B77" s="135"/>
@@ -9579,7 +9567,7 @@
       <c r="BD77" s="89"/>
     </row>
     <row r="78" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="242"/>
+      <c r="A78" s="265"/>
       <c r="B78" s="135"/>
       <c r="C78" s="90" t="s">
         <v>95</v>
@@ -9707,7 +9695,7 @@
       <c r="BD79" s="89"/>
     </row>
     <row r="80" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="240" t="s">
+      <c r="A80" s="262" t="s">
         <v>162</v>
       </c>
       <c r="B80" s="135"/>
@@ -9775,7 +9763,7 @@
       <c r="BD80" s="89"/>
     </row>
     <row r="81" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="242"/>
+      <c r="A81" s="265"/>
       <c r="B81" s="135"/>
       <c r="C81" s="90" t="s">
         <v>93</v>
@@ -9903,7 +9891,7 @@
       <c r="BD82" s="89"/>
     </row>
     <row r="83" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="240" t="s">
+      <c r="A83" s="262" t="s">
         <v>162</v>
       </c>
       <c r="B83" s="135"/>
@@ -9971,7 +9959,7 @@
       <c r="BD83" s="89"/>
     </row>
     <row r="84" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="242"/>
+      <c r="A84" s="265"/>
       <c r="B84" s="135"/>
       <c r="C84" s="90" t="s">
         <v>134</v>
@@ -10161,7 +10149,7 @@
       <c r="BD86" s="89"/>
     </row>
     <row r="87" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="240" t="s">
+      <c r="A87" s="262" t="s">
         <v>319</v>
       </c>
       <c r="B87" s="135"/>
@@ -10229,7 +10217,7 @@
       <c r="BD87" s="89"/>
     </row>
     <row r="88" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="241"/>
+      <c r="A88" s="263"/>
       <c r="B88" s="135"/>
       <c r="C88" s="95" t="s">
         <v>119</v>
@@ -10295,7 +10283,7 @@
       <c r="BD88" s="89"/>
     </row>
     <row r="89" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="241"/>
+      <c r="A89" s="263"/>
       <c r="B89" s="135"/>
       <c r="C89" s="95" t="s">
         <v>120</v>
@@ -10361,7 +10349,7 @@
       <c r="BD89" s="89"/>
     </row>
     <row r="90" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="241"/>
+      <c r="A90" s="263"/>
       <c r="B90" s="135"/>
       <c r="C90" s="95" t="s">
         <v>121</v>
@@ -10427,7 +10415,7 @@
       <c r="BD90" s="89"/>
     </row>
     <row r="91" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="241"/>
+      <c r="A91" s="263"/>
       <c r="B91" s="135"/>
       <c r="C91" s="95" t="s">
         <v>122</v>
@@ -10493,7 +10481,7 @@
       <c r="BD91" s="89"/>
     </row>
     <row r="92" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="241"/>
+      <c r="A92" s="263"/>
       <c r="B92" s="135"/>
       <c r="C92" s="95" t="s">
         <v>123</v>
@@ -10559,7 +10547,7 @@
       <c r="BD92" s="89"/>
     </row>
     <row r="93" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="241"/>
+      <c r="A93" s="263"/>
       <c r="B93" s="135"/>
       <c r="C93" s="95" t="s">
         <v>124</v>
@@ -10625,7 +10613,7 @@
       <c r="BD93" s="89"/>
     </row>
     <row r="94" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="241"/>
+      <c r="A94" s="263"/>
       <c r="B94" s="135"/>
       <c r="C94" s="95" t="s">
         <v>125</v>
@@ -10691,7 +10679,7 @@
       <c r="BD94" s="89"/>
     </row>
     <row r="95" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="241"/>
+      <c r="A95" s="263"/>
       <c r="B95" s="135"/>
       <c r="C95" s="95" t="s">
         <v>126</v>
@@ -10757,7 +10745,7 @@
       <c r="BD95" s="89"/>
     </row>
     <row r="96" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="241"/>
+      <c r="A96" s="263"/>
       <c r="B96" s="135"/>
       <c r="C96" s="95" t="s">
         <v>127</v>
@@ -10823,7 +10811,7 @@
       <c r="BD96" s="89"/>
     </row>
     <row r="97" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="241"/>
+      <c r="A97" s="263"/>
       <c r="B97" s="135"/>
       <c r="C97" s="95" t="s">
         <v>128</v>
@@ -10889,7 +10877,7 @@
       <c r="BD97" s="89"/>
     </row>
     <row r="98" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="241"/>
+      <c r="A98" s="263"/>
       <c r="B98" s="135"/>
       <c r="C98" s="95" t="s">
         <v>129</v>
@@ -10955,7 +10943,7 @@
       <c r="BD98" s="89"/>
     </row>
     <row r="99" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="241"/>
+      <c r="A99" s="263"/>
       <c r="B99" s="135"/>
       <c r="C99" s="95" t="s">
         <v>130</v>
@@ -11021,7 +11009,7 @@
       <c r="BD99" s="89"/>
     </row>
     <row r="100" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="241"/>
+      <c r="A100" s="263"/>
       <c r="B100" s="135"/>
       <c r="C100" s="95" t="s">
         <v>131</v>
@@ -11087,7 +11075,7 @@
       <c r="BD100" s="89"/>
     </row>
     <row r="101" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="241"/>
+      <c r="A101" s="263"/>
       <c r="B101" s="135"/>
       <c r="C101" s="95" t="s">
         <v>132</v>
@@ -11153,7 +11141,7 @@
       <c r="BD101" s="89"/>
     </row>
     <row r="102" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="242"/>
+      <c r="A102" s="265"/>
       <c r="B102" s="135"/>
       <c r="C102" s="95" t="s">
         <v>133</v>
@@ -11281,7 +11269,7 @@
       <c r="BD103" s="89"/>
     </row>
     <row r="104" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="240" t="s">
+      <c r="A104" s="262" t="s">
         <v>318</v>
       </c>
       <c r="B104" s="136" t="s">
@@ -11345,7 +11333,7 @@
       <c r="BD104" s="89"/>
     </row>
     <row r="105" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="241"/>
+      <c r="A105" s="263"/>
       <c r="B105" s="137">
         <v>3.0101010000000001</v>
       </c>
@@ -11413,7 +11401,7 @@
       <c r="BD105" s="89"/>
     </row>
     <row r="106" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="241"/>
+      <c r="A106" s="263"/>
       <c r="B106" s="136" t="s">
         <v>224</v>
       </c>
@@ -11475,7 +11463,7 @@
       <c r="BD106" s="89"/>
     </row>
     <row r="107" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="241"/>
+      <c r="A107" s="263"/>
       <c r="B107" s="137" t="s">
         <v>164</v>
       </c>
@@ -11543,7 +11531,7 @@
       <c r="BD107" s="89"/>
     </row>
     <row r="108" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="241"/>
+      <c r="A108" s="263"/>
       <c r="B108" s="137" t="s">
         <v>165</v>
       </c>
@@ -11611,7 +11599,7 @@
       <c r="BD108" s="89"/>
     </row>
     <row r="109" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="241"/>
+      <c r="A109" s="263"/>
       <c r="B109" s="136" t="s">
         <v>225</v>
       </c>
@@ -11673,7 +11661,7 @@
       <c r="BD109" s="89"/>
     </row>
     <row r="110" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="241"/>
+      <c r="A110" s="263"/>
       <c r="B110" s="137" t="s">
         <v>226</v>
       </c>
@@ -11741,7 +11729,7 @@
       <c r="BD110" s="89"/>
     </row>
     <row r="111" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="241"/>
+      <c r="A111" s="263"/>
       <c r="B111" s="136" t="s">
         <v>227</v>
       </c>
@@ -11803,7 +11791,7 @@
       <c r="BD111" s="89"/>
     </row>
     <row r="112" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="241"/>
+      <c r="A112" s="263"/>
       <c r="B112" s="137" t="s">
         <v>228</v>
       </c>
@@ -11871,7 +11859,7 @@
       <c r="BD112" s="89"/>
     </row>
     <row r="113" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="241"/>
+      <c r="A113" s="263"/>
       <c r="B113" s="135"/>
       <c r="C113" s="90" t="s">
         <v>174</v>
@@ -11937,7 +11925,7 @@
       <c r="BD113" s="89"/>
     </row>
     <row r="114" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="241"/>
+      <c r="A114" s="263"/>
       <c r="B114" s="135"/>
       <c r="C114" s="90" t="s">
         <v>173</v>
@@ -12003,7 +11991,7 @@
       <c r="BD114" s="89"/>
     </row>
     <row r="115" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="241"/>
+      <c r="A115" s="263"/>
       <c r="B115" s="136" t="s">
         <v>229</v>
       </c>
@@ -12065,7 +12053,7 @@
       <c r="BD115" s="89"/>
     </row>
     <row r="116" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="241"/>
+      <c r="A116" s="263"/>
       <c r="B116" s="137" t="s">
         <v>230</v>
       </c>
@@ -12133,7 +12121,7 @@
       <c r="BD116" s="89"/>
     </row>
     <row r="117" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="241"/>
+      <c r="A117" s="263"/>
       <c r="B117" s="137" t="s">
         <v>231</v>
       </c>
@@ -12201,7 +12189,7 @@
       <c r="BD117" s="89"/>
     </row>
     <row r="118" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="241"/>
+      <c r="A118" s="263"/>
       <c r="B118" s="137" t="s">
         <v>232</v>
       </c>
@@ -12269,7 +12257,7 @@
       <c r="BD118" s="89"/>
     </row>
     <row r="119" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="241"/>
+      <c r="A119" s="263"/>
       <c r="B119" s="137" t="s">
         <v>233</v>
       </c>
@@ -12337,7 +12325,7 @@
       <c r="BD119" s="89"/>
     </row>
     <row r="120" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="241"/>
+      <c r="A120" s="263"/>
       <c r="B120" s="136" t="s">
         <v>234</v>
       </c>
@@ -12399,7 +12387,7 @@
       <c r="BD120" s="89"/>
     </row>
     <row r="121" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="241"/>
+      <c r="A121" s="263"/>
       <c r="B121" s="137" t="s">
         <v>235</v>
       </c>
@@ -12467,7 +12455,7 @@
       <c r="BD121" s="89"/>
     </row>
     <row r="122" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="241"/>
+      <c r="A122" s="263"/>
       <c r="B122" s="137" t="s">
         <v>236</v>
       </c>
@@ -12535,7 +12523,7 @@
       <c r="BD122" s="89"/>
     </row>
     <row r="123" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="241"/>
+      <c r="A123" s="263"/>
       <c r="B123" s="136" t="s">
         <v>237</v>
       </c>
@@ -12597,7 +12585,7 @@
       <c r="BD123" s="89"/>
     </row>
     <row r="124" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="241"/>
+      <c r="A124" s="263"/>
       <c r="B124" s="137" t="s">
         <v>238</v>
       </c>
@@ -12661,7 +12649,7 @@
       <c r="BD124" s="89"/>
     </row>
     <row r="125" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="241"/>
+      <c r="A125" s="263"/>
       <c r="B125" s="135"/>
       <c r="C125" s="90" t="s">
         <v>183</v>
@@ -12727,7 +12715,7 @@
       <c r="BD125" s="89"/>
     </row>
     <row r="126" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="241"/>
+      <c r="A126" s="263"/>
       <c r="B126" s="135"/>
       <c r="C126" s="90" t="s">
         <v>182</v>
@@ -12793,7 +12781,7 @@
       <c r="BD126" s="89"/>
     </row>
     <row r="127" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="241"/>
+      <c r="A127" s="263"/>
       <c r="B127" s="137" t="s">
         <v>239</v>
       </c>
@@ -12857,7 +12845,7 @@
       <c r="BD127" s="89"/>
     </row>
     <row r="128" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="241"/>
+      <c r="A128" s="263"/>
       <c r="B128" s="135"/>
       <c r="C128" s="90" t="s">
         <v>282</v>
@@ -12923,7 +12911,7 @@
       <c r="BD128" s="89"/>
     </row>
     <row r="129" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="241"/>
+      <c r="A129" s="263"/>
       <c r="B129" s="135"/>
       <c r="C129" s="90" t="s">
         <v>283</v>
@@ -12989,7 +12977,7 @@
       <c r="BD129" s="89"/>
     </row>
     <row r="130" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="241"/>
+      <c r="A130" s="263"/>
       <c r="B130" s="136" t="s">
         <v>240</v>
       </c>
@@ -13051,7 +13039,7 @@
       <c r="BD130" s="89"/>
     </row>
     <row r="131" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="241"/>
+      <c r="A131" s="263"/>
       <c r="B131" s="137" t="s">
         <v>241</v>
       </c>
@@ -13119,7 +13107,7 @@
       <c r="BD131" s="89"/>
     </row>
     <row r="132" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="241"/>
+      <c r="A132" s="263"/>
       <c r="B132" s="137" t="s">
         <v>242</v>
       </c>
@@ -13187,7 +13175,7 @@
       <c r="BD132" s="89"/>
     </row>
     <row r="133" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="241"/>
+      <c r="A133" s="263"/>
       <c r="B133" s="136" t="s">
         <v>243</v>
       </c>
@@ -13249,7 +13237,7 @@
       <c r="BD133" s="89"/>
     </row>
     <row r="134" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="241"/>
+      <c r="A134" s="263"/>
       <c r="B134" s="137" t="s">
         <v>244</v>
       </c>
@@ -13317,7 +13305,7 @@
       <c r="BD134" s="89"/>
     </row>
     <row r="135" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="241"/>
+      <c r="A135" s="263"/>
       <c r="B135" s="136" t="s">
         <v>247</v>
       </c>
@@ -13379,7 +13367,7 @@
       <c r="BD135" s="89"/>
     </row>
     <row r="136" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="241"/>
+      <c r="A136" s="263"/>
       <c r="B136" s="137" t="s">
         <v>248</v>
       </c>
@@ -13447,7 +13435,7 @@
       <c r="BD136" s="89"/>
     </row>
     <row r="137" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="241"/>
+      <c r="A137" s="263"/>
       <c r="B137" s="136" t="s">
         <v>249</v>
       </c>
@@ -13509,7 +13497,7 @@
       <c r="BD137" s="89"/>
     </row>
     <row r="138" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="241"/>
+      <c r="A138" s="263"/>
       <c r="B138" s="137" t="s">
         <v>250</v>
       </c>
@@ -13577,7 +13565,7 @@
       <c r="BD138" s="89"/>
     </row>
     <row r="139" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="241"/>
+      <c r="A139" s="263"/>
       <c r="B139" s="136" t="s">
         <v>251</v>
       </c>
@@ -13639,7 +13627,7 @@
       <c r="BD139" s="89"/>
     </row>
     <row r="140" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="241"/>
+      <c r="A140" s="263"/>
       <c r="B140" s="137" t="s">
         <v>252</v>
       </c>
@@ -13707,7 +13695,7 @@
       <c r="BD140" s="89"/>
     </row>
     <row r="141" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="241"/>
+      <c r="A141" s="263"/>
       <c r="B141" s="137" t="s">
         <v>253</v>
       </c>
@@ -13775,7 +13763,7 @@
       <c r="BD141" s="89"/>
     </row>
     <row r="142" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="241"/>
+      <c r="A142" s="263"/>
       <c r="B142" s="136" t="s">
         <v>254</v>
       </c>
@@ -13837,7 +13825,7 @@
       <c r="BD142" s="89"/>
     </row>
     <row r="143" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="241"/>
+      <c r="A143" s="263"/>
       <c r="B143" s="137" t="s">
         <v>255</v>
       </c>
@@ -13905,7 +13893,7 @@
       <c r="BD143" s="89"/>
     </row>
     <row r="144" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="241"/>
+      <c r="A144" s="263"/>
       <c r="B144" s="136" t="s">
         <v>256</v>
       </c>
@@ -13967,7 +13955,7 @@
       <c r="BD144" s="89"/>
     </row>
     <row r="145" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="241"/>
+      <c r="A145" s="263"/>
       <c r="B145" s="137" t="s">
         <v>257</v>
       </c>
@@ -14035,7 +14023,7 @@
       <c r="BD145" s="89"/>
     </row>
     <row r="146" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="241"/>
+      <c r="A146" s="263"/>
       <c r="B146" s="136" t="s">
         <v>258</v>
       </c>
@@ -14097,7 +14085,7 @@
       <c r="BD146" s="89"/>
     </row>
     <row r="147" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="241"/>
+      <c r="A147" s="263"/>
       <c r="B147" s="137" t="s">
         <v>259</v>
       </c>
@@ -14165,7 +14153,7 @@
       <c r="BD147" s="89"/>
     </row>
     <row r="148" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="241"/>
+      <c r="A148" s="263"/>
       <c r="B148" s="136" t="s">
         <v>260</v>
       </c>
@@ -14227,7 +14215,7 @@
       <c r="BD148" s="89"/>
     </row>
     <row r="149" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="241"/>
+      <c r="A149" s="263"/>
       <c r="B149" s="137" t="s">
         <v>261</v>
       </c>
@@ -14295,7 +14283,7 @@
       <c r="BD149" s="89"/>
     </row>
     <row r="150" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="241"/>
+      <c r="A150" s="263"/>
       <c r="B150" s="137" t="s">
         <v>262</v>
       </c>
@@ -14363,7 +14351,7 @@
       <c r="BD150" s="89"/>
     </row>
     <row r="151" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="241"/>
+      <c r="A151" s="263"/>
       <c r="B151" s="137" t="s">
         <v>263</v>
       </c>
@@ -14431,7 +14419,7 @@
       <c r="BD151" s="89"/>
     </row>
     <row r="152" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="241"/>
+      <c r="A152" s="263"/>
       <c r="B152" s="137" t="s">
         <v>264</v>
       </c>
@@ -14499,7 +14487,7 @@
       <c r="BD152" s="89"/>
     </row>
     <row r="153" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="241"/>
+      <c r="A153" s="263"/>
       <c r="B153" s="136" t="s">
         <v>265</v>
       </c>
@@ -14561,7 +14549,7 @@
       <c r="BD153" s="89"/>
     </row>
     <row r="154" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="241"/>
+      <c r="A154" s="263"/>
       <c r="B154" s="137" t="s">
         <v>266</v>
       </c>
@@ -14629,7 +14617,7 @@
       <c r="BD154" s="89"/>
     </row>
     <row r="155" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="241"/>
+      <c r="A155" s="263"/>
       <c r="B155" s="137" t="s">
         <v>267</v>
       </c>
@@ -14697,7 +14685,7 @@
       <c r="BD155" s="89"/>
     </row>
     <row r="156" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="241"/>
+      <c r="A156" s="263"/>
       <c r="B156" s="136" t="s">
         <v>268</v>
       </c>
@@ -14759,7 +14747,7 @@
       <c r="BD156" s="89"/>
     </row>
     <row r="157" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="241"/>
+      <c r="A157" s="263"/>
       <c r="B157" s="137" t="s">
         <v>269</v>
       </c>
@@ -14827,7 +14815,7 @@
       <c r="BD157" s="89"/>
     </row>
     <row r="158" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="241"/>
+      <c r="A158" s="263"/>
       <c r="B158" s="137" t="s">
         <v>270</v>
       </c>
@@ -14895,7 +14883,7 @@
       <c r="BD158" s="89"/>
     </row>
     <row r="159" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="241"/>
+      <c r="A159" s="263"/>
       <c r="B159" s="137" t="s">
         <v>271</v>
       </c>
@@ -14963,7 +14951,7 @@
       <c r="BD159" s="89"/>
     </row>
     <row r="160" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="241"/>
+      <c r="A160" s="263"/>
       <c r="B160" s="137" t="s">
         <v>272</v>
       </c>
@@ -15031,7 +15019,7 @@
       <c r="BD160" s="89"/>
     </row>
     <row r="161" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="241"/>
+      <c r="A161" s="263"/>
       <c r="B161" s="136" t="s">
         <v>273</v>
       </c>
@@ -15093,7 +15081,7 @@
       <c r="BD161" s="89"/>
     </row>
     <row r="162" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="241"/>
+      <c r="A162" s="263"/>
       <c r="B162" s="137" t="s">
         <v>274</v>
       </c>
@@ -15161,7 +15149,7 @@
       <c r="BD162" s="89"/>
     </row>
     <row r="163" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="241"/>
+      <c r="A163" s="263"/>
       <c r="B163" s="137" t="s">
         <v>275</v>
       </c>
@@ -15229,7 +15217,7 @@
       <c r="BD163" s="89"/>
     </row>
     <row r="164" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="241"/>
+      <c r="A164" s="263"/>
       <c r="B164" s="136" t="s">
         <v>276</v>
       </c>
@@ -15291,7 +15279,7 @@
       <c r="BD164" s="89"/>
     </row>
     <row r="165" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="241"/>
+      <c r="A165" s="263"/>
       <c r="B165" s="137" t="s">
         <v>277</v>
       </c>
@@ -15359,7 +15347,7 @@
       <c r="BD165" s="89"/>
     </row>
     <row r="166" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="241"/>
+      <c r="A166" s="263"/>
       <c r="B166" s="137" t="s">
         <v>278</v>
       </c>
@@ -15427,7 +15415,7 @@
       <c r="BD166" s="89"/>
     </row>
     <row r="167" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="241"/>
+      <c r="A167" s="263"/>
       <c r="B167" s="136" t="s">
         <v>279</v>
       </c>
@@ -15489,7 +15477,7 @@
       <c r="BD167" s="89"/>
     </row>
     <row r="168" spans="1:56" s="80" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="247"/>
+      <c r="A168" s="264"/>
       <c r="B168" s="138" t="s">
         <v>280</v>
       </c>
@@ -15629,74 +15617,74 @@
         <f>SUM(K170:BD170)</f>
         <v>3500</v>
       </c>
-      <c r="E170" s="262" t="s">
+      <c r="E170" s="247" t="s">
         <v>324</v>
       </c>
-      <c r="F170" s="262"/>
-      <c r="G170" s="262"/>
-      <c r="H170" s="254"/>
-      <c r="I170" s="252"/>
-      <c r="J170" s="252"/>
-      <c r="K170" s="252">
+      <c r="F170" s="247"/>
+      <c r="G170" s="247"/>
+      <c r="H170" s="242"/>
+      <c r="I170" s="240"/>
+      <c r="J170" s="240"/>
+      <c r="K170" s="240">
         <v>500</v>
       </c>
-      <c r="L170" s="252"/>
-      <c r="M170" s="252"/>
-      <c r="N170" s="253"/>
-      <c r="O170" s="254"/>
-      <c r="P170" s="252"/>
-      <c r="Q170" s="252"/>
-      <c r="R170" s="252">
+      <c r="L170" s="240"/>
+      <c r="M170" s="240"/>
+      <c r="N170" s="241"/>
+      <c r="O170" s="242"/>
+      <c r="P170" s="240"/>
+      <c r="Q170" s="240"/>
+      <c r="R170" s="240">
         <v>500</v>
       </c>
-      <c r="S170" s="252"/>
-      <c r="T170" s="252"/>
-      <c r="U170" s="253"/>
-      <c r="V170" s="254"/>
-      <c r="W170" s="252"/>
-      <c r="X170" s="252"/>
-      <c r="Y170" s="252">
+      <c r="S170" s="240"/>
+      <c r="T170" s="240"/>
+      <c r="U170" s="241"/>
+      <c r="V170" s="242"/>
+      <c r="W170" s="240"/>
+      <c r="X170" s="240"/>
+      <c r="Y170" s="240">
         <v>500</v>
       </c>
-      <c r="Z170" s="252"/>
-      <c r="AA170" s="252"/>
-      <c r="AB170" s="253"/>
-      <c r="AC170" s="254"/>
-      <c r="AD170" s="252"/>
-      <c r="AE170" s="252"/>
-      <c r="AF170" s="252">
+      <c r="Z170" s="240"/>
+      <c r="AA170" s="240"/>
+      <c r="AB170" s="241"/>
+      <c r="AC170" s="242"/>
+      <c r="AD170" s="240"/>
+      <c r="AE170" s="240"/>
+      <c r="AF170" s="240">
         <v>500</v>
       </c>
-      <c r="AG170" s="252"/>
-      <c r="AH170" s="252"/>
-      <c r="AI170" s="253"/>
-      <c r="AJ170" s="254"/>
-      <c r="AK170" s="252"/>
-      <c r="AL170" s="252"/>
-      <c r="AM170" s="252">
+      <c r="AG170" s="240"/>
+      <c r="AH170" s="240"/>
+      <c r="AI170" s="241"/>
+      <c r="AJ170" s="242"/>
+      <c r="AK170" s="240"/>
+      <c r="AL170" s="240"/>
+      <c r="AM170" s="240">
         <v>500</v>
       </c>
-      <c r="AN170" s="252"/>
-      <c r="AO170" s="252"/>
-      <c r="AP170" s="253"/>
-      <c r="AQ170" s="254"/>
-      <c r="AR170" s="252"/>
-      <c r="AS170" s="252"/>
-      <c r="AT170" s="252">
+      <c r="AN170" s="240"/>
+      <c r="AO170" s="240"/>
+      <c r="AP170" s="241"/>
+      <c r="AQ170" s="242"/>
+      <c r="AR170" s="240"/>
+      <c r="AS170" s="240"/>
+      <c r="AT170" s="240">
         <v>500</v>
       </c>
-      <c r="AU170" s="252"/>
-      <c r="AV170" s="252"/>
-      <c r="AW170" s="253"/>
-      <c r="AX170" s="254"/>
-      <c r="AY170" s="252"/>
-      <c r="AZ170" s="252"/>
-      <c r="BA170" s="252">
+      <c r="AU170" s="240"/>
+      <c r="AV170" s="240"/>
+      <c r="AW170" s="241"/>
+      <c r="AX170" s="242"/>
+      <c r="AY170" s="240"/>
+      <c r="AZ170" s="240"/>
+      <c r="BA170" s="240">
         <v>500</v>
       </c>
-      <c r="BB170" s="252"/>
-      <c r="BC170" s="252"/>
-      <c r="BD170" s="253"/>
+      <c r="BB170" s="240"/>
+      <c r="BC170" s="240"/>
+      <c r="BD170" s="241"/>
     </row>
     <row r="171" spans="1:56" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A171" s="150"/>
@@ -15708,74 +15696,74 @@
         <f>SUM(K171:BD171)</f>
         <v>4410</v>
       </c>
-      <c r="E171" s="262" t="s">
+      <c r="E171" s="247" t="s">
         <v>323</v>
       </c>
-      <c r="F171" s="262"/>
-      <c r="G171" s="262"/>
-      <c r="H171" s="254"/>
-      <c r="I171" s="252"/>
-      <c r="J171" s="252"/>
-      <c r="K171" s="252">
+      <c r="F171" s="247"/>
+      <c r="G171" s="247"/>
+      <c r="H171" s="242"/>
+      <c r="I171" s="240"/>
+      <c r="J171" s="240"/>
+      <c r="K171" s="240">
         <v>630</v>
       </c>
-      <c r="L171" s="252"/>
-      <c r="M171" s="252"/>
-      <c r="N171" s="253"/>
-      <c r="O171" s="254"/>
-      <c r="P171" s="252"/>
-      <c r="Q171" s="252"/>
-      <c r="R171" s="252">
+      <c r="L171" s="240"/>
+      <c r="M171" s="240"/>
+      <c r="N171" s="241"/>
+      <c r="O171" s="242"/>
+      <c r="P171" s="240"/>
+      <c r="Q171" s="240"/>
+      <c r="R171" s="240">
         <v>630</v>
       </c>
-      <c r="S171" s="252"/>
-      <c r="T171" s="252"/>
-      <c r="U171" s="253"/>
-      <c r="V171" s="254"/>
-      <c r="W171" s="252"/>
-      <c r="X171" s="252"/>
-      <c r="Y171" s="252">
+      <c r="S171" s="240"/>
+      <c r="T171" s="240"/>
+      <c r="U171" s="241"/>
+      <c r="V171" s="242"/>
+      <c r="W171" s="240"/>
+      <c r="X171" s="240"/>
+      <c r="Y171" s="240">
         <v>630</v>
       </c>
-      <c r="Z171" s="252"/>
-      <c r="AA171" s="252"/>
-      <c r="AB171" s="253"/>
-      <c r="AC171" s="254"/>
-      <c r="AD171" s="252"/>
-      <c r="AE171" s="252"/>
-      <c r="AF171" s="252">
+      <c r="Z171" s="240"/>
+      <c r="AA171" s="240"/>
+      <c r="AB171" s="241"/>
+      <c r="AC171" s="242"/>
+      <c r="AD171" s="240"/>
+      <c r="AE171" s="240"/>
+      <c r="AF171" s="240">
         <v>630</v>
       </c>
-      <c r="AG171" s="252"/>
-      <c r="AH171" s="252"/>
-      <c r="AI171" s="253"/>
-      <c r="AJ171" s="254"/>
-      <c r="AK171" s="252"/>
-      <c r="AL171" s="252"/>
-      <c r="AM171" s="252">
+      <c r="AG171" s="240"/>
+      <c r="AH171" s="240"/>
+      <c r="AI171" s="241"/>
+      <c r="AJ171" s="242"/>
+      <c r="AK171" s="240"/>
+      <c r="AL171" s="240"/>
+      <c r="AM171" s="240">
         <v>630</v>
       </c>
-      <c r="AN171" s="252"/>
-      <c r="AO171" s="252"/>
-      <c r="AP171" s="253"/>
-      <c r="AQ171" s="254"/>
-      <c r="AR171" s="252"/>
-      <c r="AS171" s="252"/>
-      <c r="AT171" s="252">
+      <c r="AN171" s="240"/>
+      <c r="AO171" s="240"/>
+      <c r="AP171" s="241"/>
+      <c r="AQ171" s="242"/>
+      <c r="AR171" s="240"/>
+      <c r="AS171" s="240"/>
+      <c r="AT171" s="240">
         <v>630</v>
       </c>
-      <c r="AU171" s="252"/>
-      <c r="AV171" s="252"/>
-      <c r="AW171" s="253"/>
-      <c r="AX171" s="254"/>
-      <c r="AY171" s="252"/>
-      <c r="AZ171" s="252"/>
-      <c r="BA171" s="252">
+      <c r="AU171" s="240"/>
+      <c r="AV171" s="240"/>
+      <c r="AW171" s="241"/>
+      <c r="AX171" s="242"/>
+      <c r="AY171" s="240"/>
+      <c r="AZ171" s="240"/>
+      <c r="BA171" s="240">
         <v>630</v>
       </c>
-      <c r="BB171" s="252"/>
-      <c r="BC171" s="252"/>
-      <c r="BD171" s="253"/>
+      <c r="BB171" s="240"/>
+      <c r="BC171" s="240"/>
+      <c r="BD171" s="241"/>
     </row>
     <row r="172" spans="1:56" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="152"/>
@@ -15787,74 +15775,74 @@
         <f>+D169+D171</f>
         <v>9910</v>
       </c>
-      <c r="E172" s="255" t="s">
+      <c r="E172" s="256" t="s">
         <v>307</v>
       </c>
-      <c r="F172" s="255"/>
-      <c r="G172" s="255"/>
-      <c r="H172" s="250"/>
-      <c r="I172" s="251"/>
-      <c r="J172" s="251"/>
-      <c r="K172" s="248">
+      <c r="F172" s="256"/>
+      <c r="G172" s="256"/>
+      <c r="H172" s="258"/>
+      <c r="I172" s="259"/>
+      <c r="J172" s="259"/>
+      <c r="K172" s="260">
         <v>44607</v>
       </c>
-      <c r="L172" s="248"/>
-      <c r="M172" s="248"/>
-      <c r="N172" s="249"/>
-      <c r="O172" s="250"/>
-      <c r="P172" s="251"/>
-      <c r="Q172" s="251"/>
-      <c r="R172" s="248">
+      <c r="L172" s="260"/>
+      <c r="M172" s="260"/>
+      <c r="N172" s="261"/>
+      <c r="O172" s="258"/>
+      <c r="P172" s="259"/>
+      <c r="Q172" s="259"/>
+      <c r="R172" s="260">
         <v>44607</v>
       </c>
-      <c r="S172" s="248"/>
-      <c r="T172" s="248"/>
-      <c r="U172" s="249"/>
-      <c r="V172" s="250"/>
-      <c r="W172" s="251"/>
-      <c r="X172" s="251"/>
-      <c r="Y172" s="248">
+      <c r="S172" s="260"/>
+      <c r="T172" s="260"/>
+      <c r="U172" s="261"/>
+      <c r="V172" s="258"/>
+      <c r="W172" s="259"/>
+      <c r="X172" s="259"/>
+      <c r="Y172" s="260">
         <v>44607</v>
       </c>
-      <c r="Z172" s="248"/>
-      <c r="AA172" s="248"/>
-      <c r="AB172" s="249"/>
-      <c r="AC172" s="250"/>
-      <c r="AD172" s="251"/>
-      <c r="AE172" s="251"/>
-      <c r="AF172" s="248">
+      <c r="Z172" s="260"/>
+      <c r="AA172" s="260"/>
+      <c r="AB172" s="261"/>
+      <c r="AC172" s="258"/>
+      <c r="AD172" s="259"/>
+      <c r="AE172" s="259"/>
+      <c r="AF172" s="260">
         <v>44607</v>
       </c>
-      <c r="AG172" s="248"/>
-      <c r="AH172" s="248"/>
-      <c r="AI172" s="249"/>
-      <c r="AJ172" s="250"/>
-      <c r="AK172" s="251"/>
-      <c r="AL172" s="251"/>
-      <c r="AM172" s="248">
+      <c r="AG172" s="260"/>
+      <c r="AH172" s="260"/>
+      <c r="AI172" s="261"/>
+      <c r="AJ172" s="258"/>
+      <c r="AK172" s="259"/>
+      <c r="AL172" s="259"/>
+      <c r="AM172" s="260">
         <v>44607</v>
       </c>
-      <c r="AN172" s="248"/>
-      <c r="AO172" s="248"/>
-      <c r="AP172" s="249"/>
-      <c r="AQ172" s="250"/>
-      <c r="AR172" s="251"/>
-      <c r="AS172" s="251"/>
-      <c r="AT172" s="248">
+      <c r="AN172" s="260"/>
+      <c r="AO172" s="260"/>
+      <c r="AP172" s="261"/>
+      <c r="AQ172" s="258"/>
+      <c r="AR172" s="259"/>
+      <c r="AS172" s="259"/>
+      <c r="AT172" s="260">
         <v>44607</v>
       </c>
-      <c r="AU172" s="248"/>
-      <c r="AV172" s="248"/>
-      <c r="AW172" s="249"/>
-      <c r="AX172" s="250"/>
-      <c r="AY172" s="251"/>
-      <c r="AZ172" s="251"/>
-      <c r="BA172" s="248">
+      <c r="AU172" s="260"/>
+      <c r="AV172" s="260"/>
+      <c r="AW172" s="261"/>
+      <c r="AX172" s="258"/>
+      <c r="AY172" s="259"/>
+      <c r="AZ172" s="259"/>
+      <c r="BA172" s="260">
         <v>44607</v>
       </c>
-      <c r="BB172" s="248"/>
-      <c r="BC172" s="248"/>
-      <c r="BD172" s="249"/>
+      <c r="BB172" s="260"/>
+      <c r="BC172" s="260"/>
+      <c r="BD172" s="261"/>
     </row>
     <row r="173" spans="1:56" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="163"/>
@@ -15979,6 +15967,75 @@
     </row>
   </sheetData>
   <mergeCells count="85">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="AJ6:AP6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A15:A30"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="O6:U6"/>
+    <mergeCell ref="V6:AB6"/>
+    <mergeCell ref="AC6:AI6"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A104:A168"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A87:A102"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A37:A74"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="R172:U172"/>
+    <mergeCell ref="V172:X172"/>
+    <mergeCell ref="Y170:AB170"/>
+    <mergeCell ref="AC170:AE170"/>
+    <mergeCell ref="AF170:AI170"/>
+    <mergeCell ref="V170:X170"/>
+    <mergeCell ref="R170:U170"/>
+    <mergeCell ref="AQ172:AS172"/>
+    <mergeCell ref="AT172:AW172"/>
+    <mergeCell ref="AX172:AZ172"/>
+    <mergeCell ref="BA172:BD172"/>
+    <mergeCell ref="Y172:AB172"/>
+    <mergeCell ref="AC172:AE172"/>
+    <mergeCell ref="AF172:AI172"/>
+    <mergeCell ref="AJ172:AL172"/>
+    <mergeCell ref="AM172:AP172"/>
+    <mergeCell ref="E172:G172"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="I3:Q3"/>
+    <mergeCell ref="I4:Q4"/>
+    <mergeCell ref="H172:J172"/>
+    <mergeCell ref="K172:N172"/>
+    <mergeCell ref="O172:Q172"/>
+    <mergeCell ref="H170:J170"/>
+    <mergeCell ref="K170:N170"/>
+    <mergeCell ref="O170:Q170"/>
+    <mergeCell ref="AL1:BD1"/>
+    <mergeCell ref="O1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="E171:G171"/>
+    <mergeCell ref="H171:J171"/>
+    <mergeCell ref="K171:N171"/>
+    <mergeCell ref="O171:Q171"/>
+    <mergeCell ref="R171:U171"/>
+    <mergeCell ref="V171:X171"/>
+    <mergeCell ref="Y171:AB171"/>
+    <mergeCell ref="AC171:AE171"/>
+    <mergeCell ref="AF171:AI171"/>
+    <mergeCell ref="AJ171:AL171"/>
+    <mergeCell ref="AM171:AP171"/>
+    <mergeCell ref="AQ171:AS171"/>
     <mergeCell ref="AT171:AW171"/>
     <mergeCell ref="AX171:AZ171"/>
     <mergeCell ref="BA171:BD171"/>
@@ -15995,75 +16052,6 @@
     <mergeCell ref="AQ170:AS170"/>
     <mergeCell ref="AQ6:AW6"/>
     <mergeCell ref="AX6:BD6"/>
-    <mergeCell ref="AL1:BD1"/>
-    <mergeCell ref="O1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="E171:G171"/>
-    <mergeCell ref="H171:J171"/>
-    <mergeCell ref="K171:N171"/>
-    <mergeCell ref="O171:Q171"/>
-    <mergeCell ref="R171:U171"/>
-    <mergeCell ref="V171:X171"/>
-    <mergeCell ref="Y171:AB171"/>
-    <mergeCell ref="AC171:AE171"/>
-    <mergeCell ref="AF171:AI171"/>
-    <mergeCell ref="AJ171:AL171"/>
-    <mergeCell ref="AM171:AP171"/>
-    <mergeCell ref="AQ171:AS171"/>
-    <mergeCell ref="E172:G172"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="I3:Q3"/>
-    <mergeCell ref="I4:Q4"/>
-    <mergeCell ref="H172:J172"/>
-    <mergeCell ref="K172:N172"/>
-    <mergeCell ref="O172:Q172"/>
-    <mergeCell ref="H170:J170"/>
-    <mergeCell ref="K170:N170"/>
-    <mergeCell ref="O170:Q170"/>
-    <mergeCell ref="AQ172:AS172"/>
-    <mergeCell ref="AT172:AW172"/>
-    <mergeCell ref="AX172:AZ172"/>
-    <mergeCell ref="BA172:BD172"/>
-    <mergeCell ref="Y172:AB172"/>
-    <mergeCell ref="AC172:AE172"/>
-    <mergeCell ref="AF172:AI172"/>
-    <mergeCell ref="AJ172:AL172"/>
-    <mergeCell ref="AM172:AP172"/>
-    <mergeCell ref="R172:U172"/>
-    <mergeCell ref="V172:X172"/>
-    <mergeCell ref="Y170:AB170"/>
-    <mergeCell ref="AC170:AE170"/>
-    <mergeCell ref="AF170:AI170"/>
-    <mergeCell ref="V170:X170"/>
-    <mergeCell ref="R170:U170"/>
-    <mergeCell ref="A104:A168"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="A87:A102"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A37:A74"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="AJ6:AP6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A15:A30"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="O6:U6"/>
-    <mergeCell ref="V6:AB6"/>
-    <mergeCell ref="AC6:AI6"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -16083,42 +16071,41 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AH36"/>
+  <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A12" zoomScale="129" zoomScaleNormal="129" zoomScaleSheetLayoutView="129" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35:H35"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="129" zoomScaleNormal="129" zoomScaleSheetLayoutView="129" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="190" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="180" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" style="180" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="180" customWidth="1"/>
-    <col min="5" max="6" width="10.28515625" style="180" customWidth="1"/>
-    <col min="7" max="9" width="9.28515625" style="180" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" style="180" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="180" customWidth="1"/>
-    <col min="12" max="12" width="4.7109375" style="180" customWidth="1"/>
-    <col min="13" max="16" width="5.7109375" style="180" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="180" bestFit="1" customWidth="1"/>
-    <col min="18" max="30" width="5.7109375" style="180" customWidth="1"/>
-    <col min="31" max="31" width="11.42578125" style="180"/>
-    <col min="32" max="32" width="18.42578125" style="180" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="11.42578125" style="180"/>
+    <col min="3" max="3" width="65" style="180" customWidth="1"/>
+    <col min="4" max="5" width="10.28515625" style="180" customWidth="1"/>
+    <col min="6" max="8" width="9.28515625" style="180" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="180" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="180" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" style="180" customWidth="1"/>
+    <col min="12" max="15" width="5.7109375" style="180" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="180" bestFit="1" customWidth="1"/>
+    <col min="17" max="29" width="5.7109375" style="180" customWidth="1"/>
+    <col min="30" max="30" width="11.42578125" style="180"/>
+    <col min="31" max="31" width="18.42578125" style="180" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="11.42578125" style="180"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="277" t="s">
+    <row r="1" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="300" t="s">
         <v>355</v>
       </c>
-      <c r="D1" s="277"/>
-      <c r="E1" s="277"/>
-      <c r="F1" s="277"/>
-      <c r="G1" s="277"/>
-      <c r="H1" s="277"/>
-      <c r="I1" s="277"/>
-      <c r="J1" s="277"/>
+      <c r="D1" s="300"/>
+      <c r="E1" s="300"/>
+      <c r="F1" s="300"/>
+      <c r="G1" s="300"/>
+      <c r="H1" s="300"/>
+      <c r="I1" s="300"/>
+      <c r="J1" s="207"/>
       <c r="K1" s="207"/>
       <c r="L1" s="207"/>
       <c r="M1" s="207"/>
@@ -16138,22 +16125,21 @@
       <c r="AA1" s="207"/>
       <c r="AB1" s="207"/>
       <c r="AC1" s="207"/>
-      <c r="AD1" s="207"/>
+      <c r="AD1" s="181"/>
       <c r="AE1" s="181"/>
       <c r="AF1" s="181"/>
       <c r="AG1" s="181"/>
-      <c r="AH1" s="181"/>
-    </row>
-    <row r="2" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="207"/>
-      <c r="C2" s="277"/>
-      <c r="D2" s="277"/>
-      <c r="E2" s="277"/>
-      <c r="F2" s="277"/>
-      <c r="G2" s="277"/>
-      <c r="H2" s="277"/>
-      <c r="I2" s="277"/>
-      <c r="J2" s="277"/>
+      <c r="C2" s="300"/>
+      <c r="D2" s="300"/>
+      <c r="E2" s="300"/>
+      <c r="F2" s="300"/>
+      <c r="G2" s="300"/>
+      <c r="H2" s="300"/>
+      <c r="I2" s="300"/>
+      <c r="J2" s="207"/>
       <c r="K2" s="207"/>
       <c r="L2" s="207"/>
       <c r="M2" s="207"/>
@@ -16173,21 +16159,20 @@
       <c r="AA2" s="207"/>
       <c r="AB2" s="207"/>
       <c r="AC2" s="207"/>
-      <c r="AD2" s="207"/>
+      <c r="AD2" s="181"/>
       <c r="AE2" s="181"/>
       <c r="AF2" s="181"/>
       <c r="AG2" s="181"/>
-      <c r="AH2" s="181"/>
-    </row>
-    <row r="3" spans="2:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="206"/>
       <c r="C3" s="206"/>
       <c r="D3" s="206"/>
       <c r="E3" s="206"/>
       <c r="F3" s="206"/>
-      <c r="G3" s="206"/>
+      <c r="G3" s="205"/>
       <c r="H3" s="205"/>
-      <c r="I3" s="205"/>
+      <c r="I3" s="207"/>
       <c r="J3" s="207"/>
       <c r="K3" s="207"/>
       <c r="L3" s="207"/>
@@ -16208,26 +16193,25 @@
       <c r="AA3" s="207"/>
       <c r="AB3" s="207"/>
       <c r="AC3" s="207"/>
-      <c r="AD3" s="207"/>
+      <c r="AD3" s="181"/>
       <c r="AE3" s="181"/>
       <c r="AF3" s="181"/>
       <c r="AG3" s="181"/>
-      <c r="AH3" s="181"/>
-    </row>
-    <row r="4" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="205"/>
-      <c r="C4" s="282" t="s">
-        <v>364</v>
-      </c>
-      <c r="D4" s="283"/>
-      <c r="E4" s="284" t="s">
-        <v>366</v>
-      </c>
-      <c r="F4" s="284"/>
-      <c r="G4" s="284"/>
-      <c r="H4" s="284"/>
-      <c r="I4" s="284"/>
-      <c r="J4" s="285"/>
+      <c r="C4" s="229" t="s">
+        <v>363</v>
+      </c>
+      <c r="D4" s="296" t="s">
+        <v>365</v>
+      </c>
+      <c r="E4" s="296"/>
+      <c r="F4" s="296"/>
+      <c r="G4" s="296"/>
+      <c r="H4" s="296"/>
+      <c r="I4" s="297"/>
+      <c r="J4" s="207"/>
       <c r="K4" s="207"/>
       <c r="L4" s="207"/>
       <c r="M4" s="207"/>
@@ -16247,26 +16231,25 @@
       <c r="AA4" s="207"/>
       <c r="AB4" s="207"/>
       <c r="AC4" s="207"/>
-      <c r="AD4" s="207"/>
+      <c r="AD4" s="181"/>
       <c r="AE4" s="181"/>
       <c r="AF4" s="181"/>
       <c r="AG4" s="181"/>
-      <c r="AH4" s="181"/>
-    </row>
-    <row r="5" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="190"/>
-      <c r="C5" s="282" t="s">
-        <v>365</v>
-      </c>
-      <c r="D5" s="283"/>
-      <c r="E5" s="299" t="s">
-        <v>367</v>
-      </c>
-      <c r="F5" s="299"/>
-      <c r="G5" s="299"/>
-      <c r="H5" s="299"/>
-      <c r="I5" s="299"/>
-      <c r="J5" s="300"/>
+      <c r="C5" s="229" t="s">
+        <v>364</v>
+      </c>
+      <c r="D5" s="305" t="s">
+        <v>366</v>
+      </c>
+      <c r="E5" s="305"/>
+      <c r="F5" s="305"/>
+      <c r="G5" s="305"/>
+      <c r="H5" s="305"/>
+      <c r="I5" s="306"/>
+      <c r="J5" s="207"/>
       <c r="K5" s="207"/>
       <c r="L5" s="207"/>
       <c r="M5" s="207"/>
@@ -16286,13 +16269,12 @@
       <c r="AA5" s="207"/>
       <c r="AB5" s="207"/>
       <c r="AC5" s="207"/>
-      <c r="AD5" s="207"/>
+      <c r="AD5" s="181"/>
       <c r="AE5" s="181"/>
       <c r="AF5" s="181"/>
       <c r="AG5" s="181"/>
-      <c r="AH5" s="181"/>
-    </row>
-    <row r="6" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="190"/>
       <c r="C6" s="190"/>
       <c r="D6" s="190"/>
@@ -16301,7 +16283,7 @@
       <c r="G6" s="190"/>
       <c r="H6" s="190"/>
       <c r="I6" s="190"/>
-      <c r="J6" s="190"/>
+      <c r="J6" s="207"/>
       <c r="K6" s="207"/>
       <c r="L6" s="207"/>
       <c r="M6" s="207"/>
@@ -16321,26 +16303,25 @@
       <c r="AA6" s="207"/>
       <c r="AB6" s="207"/>
       <c r="AC6" s="207"/>
-      <c r="AD6" s="207"/>
+      <c r="AD6" s="181"/>
       <c r="AE6" s="181"/>
       <c r="AF6" s="181"/>
       <c r="AG6" s="181"/>
-      <c r="AH6" s="181"/>
-    </row>
-    <row r="7" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="190"/>
-      <c r="C7" s="282" t="s">
+      <c r="C7" s="229" t="s">
         <v>294</v>
       </c>
-      <c r="D7" s="283"/>
-      <c r="E7" s="284" t="s">
-        <v>369</v>
-      </c>
-      <c r="F7" s="284"/>
-      <c r="G7" s="284"/>
-      <c r="H7" s="284"/>
-      <c r="I7" s="284"/>
-      <c r="J7" s="285"/>
+      <c r="D7" s="296" t="s">
+        <v>368</v>
+      </c>
+      <c r="E7" s="296"/>
+      <c r="F7" s="296"/>
+      <c r="G7" s="296"/>
+      <c r="H7" s="296"/>
+      <c r="I7" s="297"/>
+      <c r="J7" s="207"/>
       <c r="K7" s="207"/>
       <c r="L7" s="207"/>
       <c r="M7" s="207"/>
@@ -16360,26 +16341,25 @@
       <c r="AA7" s="207"/>
       <c r="AB7" s="207"/>
       <c r="AC7" s="207"/>
-      <c r="AD7" s="207"/>
+      <c r="AD7" s="181"/>
       <c r="AE7" s="181"/>
       <c r="AF7" s="181"/>
       <c r="AG7" s="181"/>
-      <c r="AH7" s="181"/>
-    </row>
-    <row r="8" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="205"/>
-      <c r="C8" s="282" t="s">
+      <c r="C8" s="229" t="s">
         <v>342</v>
       </c>
-      <c r="D8" s="283"/>
-      <c r="E8" s="284" t="s">
+      <c r="D8" s="296" t="s">
         <v>346</v>
       </c>
-      <c r="F8" s="284"/>
-      <c r="G8" s="284"/>
-      <c r="H8" s="284"/>
-      <c r="I8" s="284"/>
-      <c r="J8" s="285"/>
+      <c r="E8" s="296"/>
+      <c r="F8" s="296"/>
+      <c r="G8" s="296"/>
+      <c r="H8" s="296"/>
+      <c r="I8" s="297"/>
+      <c r="J8" s="207"/>
       <c r="K8" s="207"/>
       <c r="L8" s="207"/>
       <c r="M8" s="207"/>
@@ -16399,25 +16379,24 @@
       <c r="AA8" s="207"/>
       <c r="AB8" s="207"/>
       <c r="AC8" s="207"/>
-      <c r="AD8" s="207"/>
+      <c r="AD8" s="181"/>
       <c r="AE8" s="181"/>
       <c r="AF8" s="181"/>
       <c r="AG8" s="181"/>
-      <c r="AH8" s="181"/>
-    </row>
-    <row r="9" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="205"/>
-      <c r="C9" s="282" t="s">
-        <v>357</v>
-      </c>
-      <c r="D9" s="283"/>
-      <c r="E9" s="284"/>
-      <c r="F9" s="284"/>
-      <c r="G9" s="284"/>
-      <c r="H9" s="284"/>
-      <c r="I9" s="284"/>
-      <c r="J9" s="285"/>
-      <c r="K9" s="226"/>
+      <c r="C9" s="229" t="s">
+        <v>356</v>
+      </c>
+      <c r="D9" s="296"/>
+      <c r="E9" s="296"/>
+      <c r="F9" s="296"/>
+      <c r="G9" s="296"/>
+      <c r="H9" s="296"/>
+      <c r="I9" s="297"/>
+      <c r="J9" s="226"/>
+      <c r="K9" s="207"/>
       <c r="L9" s="207"/>
       <c r="M9" s="207"/>
       <c r="N9" s="207"/>
@@ -16436,26 +16415,25 @@
       <c r="AA9" s="207"/>
       <c r="AB9" s="207"/>
       <c r="AC9" s="207"/>
-      <c r="AD9" s="207"/>
+      <c r="AD9" s="181"/>
       <c r="AE9" s="181"/>
       <c r="AF9" s="181"/>
       <c r="AG9" s="181"/>
-      <c r="AH9" s="181"/>
-    </row>
-    <row r="10" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="205"/>
-      <c r="C10" s="282" t="s">
-        <v>363</v>
-      </c>
-      <c r="D10" s="283"/>
-      <c r="E10" s="301" t="s">
+      <c r="C10" s="229" t="s">
+        <v>362</v>
+      </c>
+      <c r="D10" s="307" t="s">
         <v>353</v>
       </c>
-      <c r="F10" s="301"/>
-      <c r="G10" s="301"/>
-      <c r="H10" s="301"/>
-      <c r="I10" s="301"/>
-      <c r="J10" s="302"/>
+      <c r="E10" s="307"/>
+      <c r="F10" s="307"/>
+      <c r="G10" s="307"/>
+      <c r="H10" s="307"/>
+      <c r="I10" s="308"/>
+      <c r="J10" s="207"/>
       <c r="K10" s="207"/>
       <c r="L10" s="207"/>
       <c r="M10" s="207"/>
@@ -16475,21 +16453,20 @@
       <c r="AA10" s="207"/>
       <c r="AB10" s="207"/>
       <c r="AC10" s="207"/>
-      <c r="AD10" s="207"/>
+      <c r="AD10" s="181"/>
       <c r="AE10" s="181"/>
       <c r="AF10" s="181"/>
       <c r="AG10" s="181"/>
-      <c r="AH10" s="181"/>
-    </row>
-    <row r="11" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="205"/>
       <c r="C11" s="208"/>
-      <c r="D11" s="208"/>
+      <c r="D11" s="189"/>
       <c r="E11" s="189"/>
       <c r="F11" s="189"/>
       <c r="G11" s="189"/>
-      <c r="H11" s="189"/>
-      <c r="I11" s="205"/>
+      <c r="H11" s="205"/>
+      <c r="I11" s="207"/>
       <c r="J11" s="207"/>
       <c r="K11" s="207"/>
       <c r="L11" s="207"/>
@@ -16510,26 +16487,23 @@
       <c r="AA11" s="207"/>
       <c r="AB11" s="207"/>
       <c r="AC11" s="207"/>
-      <c r="AD11" s="207"/>
+      <c r="AD11" s="181"/>
       <c r="AE11" s="181"/>
       <c r="AF11" s="181"/>
       <c r="AG11" s="181"/>
-      <c r="AH11" s="181"/>
-    </row>
-    <row r="12" spans="2:34" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:33" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="190"/>
       <c r="C12" s="216" t="s">
-        <v>370</v>
-      </c>
-      <c r="D12" s="284" t="s">
-        <v>356</v>
-      </c>
-      <c r="E12" s="284"/>
-      <c r="F12" s="284"/>
-      <c r="G12" s="284"/>
-      <c r="H12" s="284"/>
-      <c r="I12" s="284"/>
-      <c r="J12" s="285"/>
+        <v>369</v>
+      </c>
+      <c r="D12" s="296"/>
+      <c r="E12" s="296"/>
+      <c r="F12" s="296"/>
+      <c r="G12" s="296"/>
+      <c r="H12" s="296"/>
+      <c r="I12" s="297"/>
+      <c r="J12" s="207"/>
       <c r="K12" s="207"/>
       <c r="L12" s="207"/>
       <c r="M12" s="207"/>
@@ -16549,13 +16523,12 @@
       <c r="AA12" s="207"/>
       <c r="AB12" s="207"/>
       <c r="AC12" s="207"/>
-      <c r="AD12" s="207"/>
+      <c r="AD12" s="181"/>
       <c r="AE12" s="181"/>
       <c r="AF12" s="181"/>
       <c r="AG12" s="181"/>
-      <c r="AH12" s="181"/>
-    </row>
-    <row r="13" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="190"/>
       <c r="C13" s="198"/>
       <c r="D13" s="189"/>
@@ -16564,7 +16537,7 @@
       <c r="G13" s="189"/>
       <c r="H13" s="189"/>
       <c r="I13" s="189"/>
-      <c r="J13" s="189"/>
+      <c r="J13" s="207"/>
       <c r="K13" s="207"/>
       <c r="L13" s="207"/>
       <c r="M13" s="207"/>
@@ -16584,28 +16557,27 @@
       <c r="AA13" s="207"/>
       <c r="AB13" s="207"/>
       <c r="AC13" s="207"/>
-      <c r="AD13" s="207"/>
+      <c r="AD13" s="181"/>
       <c r="AE13" s="181"/>
       <c r="AF13" s="181"/>
       <c r="AG13" s="181"/>
-      <c r="AH13" s="181"/>
-    </row>
-    <row r="14" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="190"/>
       <c r="C14" s="216" t="s">
-        <v>358</v>
-      </c>
-      <c r="D14" s="273"/>
-      <c r="E14" s="274"/>
-      <c r="F14" s="190"/>
-      <c r="G14" s="271" t="s">
-        <v>361</v>
-      </c>
-      <c r="H14" s="272"/>
-      <c r="I14" s="273"/>
-      <c r="J14" s="274"/>
+        <v>357</v>
+      </c>
+      <c r="D14" s="227"/>
+      <c r="E14" s="190"/>
+      <c r="F14" s="313" t="s">
+        <v>360</v>
+      </c>
+      <c r="G14" s="314"/>
+      <c r="H14" s="298"/>
+      <c r="I14" s="299"/>
+      <c r="J14" s="190"/>
       <c r="K14" s="190"/>
-      <c r="L14" s="190"/>
+      <c r="L14" s="207"/>
       <c r="M14" s="207"/>
       <c r="N14" s="207"/>
       <c r="O14" s="207"/>
@@ -16623,28 +16595,27 @@
       <c r="AA14" s="207"/>
       <c r="AB14" s="207"/>
       <c r="AC14" s="207"/>
-      <c r="AD14" s="207"/>
+      <c r="AD14" s="181"/>
       <c r="AE14" s="181"/>
       <c r="AF14" s="181"/>
       <c r="AG14" s="181"/>
-      <c r="AH14" s="181"/>
-    </row>
-    <row r="15" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="190"/>
       <c r="C15" s="216" t="s">
-        <v>359</v>
-      </c>
-      <c r="D15" s="273"/>
-      <c r="E15" s="274"/>
-      <c r="F15" s="190"/>
-      <c r="G15" s="271" t="s">
-        <v>362</v>
-      </c>
-      <c r="H15" s="272"/>
-      <c r="I15" s="275"/>
-      <c r="J15" s="276"/>
+        <v>358</v>
+      </c>
+      <c r="D15" s="227"/>
+      <c r="E15" s="190"/>
+      <c r="F15" s="313" t="s">
+        <v>361</v>
+      </c>
+      <c r="G15" s="314"/>
+      <c r="H15" s="309"/>
+      <c r="I15" s="310"/>
+      <c r="J15" s="190"/>
       <c r="K15" s="190"/>
-      <c r="L15" s="190"/>
+      <c r="L15" s="207"/>
       <c r="M15" s="207"/>
       <c r="N15" s="207"/>
       <c r="O15" s="207"/>
@@ -16662,19 +16633,18 @@
       <c r="AA15" s="207"/>
       <c r="AB15" s="207"/>
       <c r="AC15" s="207"/>
-      <c r="AD15" s="207"/>
-    </row>
-    <row r="16" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="190"/>
       <c r="C16" s="217" t="s">
-        <v>360</v>
-      </c>
-      <c r="D16" s="275"/>
-      <c r="E16" s="276"/>
+        <v>359</v>
+      </c>
+      <c r="D16" s="228"/>
+      <c r="E16" s="196"/>
       <c r="F16" s="196"/>
-      <c r="G16" s="196"/>
+      <c r="G16" s="190"/>
       <c r="H16" s="190"/>
-      <c r="I16" s="190"/>
+      <c r="I16" s="207"/>
       <c r="J16" s="207"/>
       <c r="K16" s="207"/>
       <c r="L16" s="207"/>
@@ -16695,17 +16665,16 @@
       <c r="AA16" s="207"/>
       <c r="AB16" s="207"/>
       <c r="AC16" s="207"/>
-      <c r="AD16" s="207"/>
-    </row>
-    <row r="17" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="190"/>
       <c r="C17" s="190"/>
       <c r="D17" s="190"/>
-      <c r="E17" s="190"/>
-      <c r="F17" s="196"/>
+      <c r="E17" s="196"/>
+      <c r="F17" s="182"/>
       <c r="G17" s="182"/>
       <c r="H17" s="182"/>
-      <c r="I17" s="182"/>
+      <c r="I17" s="207"/>
       <c r="J17" s="207"/>
       <c r="K17" s="207"/>
       <c r="L17" s="207"/>
@@ -16726,21 +16695,20 @@
       <c r="AA17" s="207"/>
       <c r="AB17" s="207"/>
       <c r="AC17" s="207"/>
-      <c r="AD17" s="207"/>
-    </row>
-    <row r="18" spans="1:34" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:33" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="190"/>
-      <c r="C18" s="278" t="s">
+      <c r="C18" s="301" t="s">
         <v>305</v>
       </c>
-      <c r="D18" s="279"/>
-      <c r="E18" s="279"/>
-      <c r="F18" s="279"/>
-      <c r="G18" s="279"/>
-      <c r="H18" s="279"/>
-      <c r="I18" s="279"/>
-      <c r="J18" s="210"/>
-      <c r="K18" s="190"/>
+      <c r="D18" s="302"/>
+      <c r="E18" s="302"/>
+      <c r="F18" s="302"/>
+      <c r="G18" s="302"/>
+      <c r="H18" s="302"/>
+      <c r="I18" s="210"/>
+      <c r="J18" s="190"/>
+      <c r="K18" s="185"/>
       <c r="L18" s="185"/>
       <c r="M18" s="185"/>
       <c r="N18" s="185"/>
@@ -16748,32 +16716,31 @@
       <c r="P18" s="185"/>
       <c r="Q18" s="185"/>
       <c r="R18" s="185"/>
-      <c r="S18" s="185"/>
+      <c r="S18" s="194"/>
       <c r="T18" s="194"/>
       <c r="U18" s="194"/>
       <c r="V18" s="194"/>
       <c r="W18" s="194"/>
       <c r="X18" s="194"/>
       <c r="Y18" s="194"/>
-      <c r="Z18" s="194"/>
+      <c r="Z18" s="193"/>
       <c r="AA18" s="193"/>
       <c r="AB18" s="193"/>
       <c r="AC18" s="193"/>
-      <c r="AD18" s="193"/>
-    </row>
-    <row r="19" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="190"/>
-      <c r="C19" s="280" t="s">
+      <c r="C19" s="303" t="s">
         <v>303</v>
       </c>
-      <c r="D19" s="281"/>
-      <c r="E19" s="281"/>
-      <c r="F19" s="281"/>
-      <c r="G19" s="281"/>
-      <c r="H19" s="281"/>
-      <c r="I19" s="281"/>
-      <c r="J19" s="210"/>
-      <c r="K19" s="190"/>
+      <c r="D19" s="304"/>
+      <c r="E19" s="304"/>
+      <c r="F19" s="304"/>
+      <c r="G19" s="304"/>
+      <c r="H19" s="304"/>
+      <c r="I19" s="210"/>
+      <c r="J19" s="190"/>
+      <c r="K19" s="185"/>
       <c r="L19" s="185"/>
       <c r="M19" s="185"/>
       <c r="N19" s="185"/>
@@ -16781,32 +16748,31 @@
       <c r="P19" s="185"/>
       <c r="Q19" s="185"/>
       <c r="R19" s="185"/>
-      <c r="S19" s="185"/>
+      <c r="S19" s="194"/>
       <c r="T19" s="194"/>
       <c r="U19" s="194"/>
       <c r="V19" s="194"/>
       <c r="W19" s="194"/>
       <c r="X19" s="194"/>
       <c r="Y19" s="194"/>
-      <c r="Z19" s="194"/>
+      <c r="Z19" s="193"/>
       <c r="AA19" s="193"/>
       <c r="AB19" s="193"/>
       <c r="AC19" s="193"/>
-      <c r="AD19" s="193"/>
-    </row>
-    <row r="20" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:33" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="190"/>
-      <c r="C20" s="269" t="s">
+      <c r="C20" s="311" t="s">
         <v>304</v>
       </c>
-      <c r="D20" s="270"/>
-      <c r="E20" s="270"/>
-      <c r="F20" s="270"/>
-      <c r="G20" s="270"/>
-      <c r="H20" s="270"/>
-      <c r="I20" s="270"/>
-      <c r="J20" s="209"/>
-      <c r="K20" s="190"/>
+      <c r="D20" s="312"/>
+      <c r="E20" s="312"/>
+      <c r="F20" s="312"/>
+      <c r="G20" s="312"/>
+      <c r="H20" s="312"/>
+      <c r="I20" s="209"/>
+      <c r="J20" s="190"/>
+      <c r="K20" s="185"/>
       <c r="L20" s="185"/>
       <c r="M20" s="185"/>
       <c r="N20" s="185"/>
@@ -16814,30 +16780,29 @@
       <c r="P20" s="185"/>
       <c r="Q20" s="185"/>
       <c r="R20" s="185"/>
-      <c r="S20" s="185"/>
+      <c r="S20" s="194"/>
       <c r="T20" s="194"/>
       <c r="U20" s="194"/>
       <c r="V20" s="194"/>
       <c r="W20" s="194"/>
       <c r="X20" s="194"/>
       <c r="Y20" s="194"/>
-      <c r="Z20" s="194"/>
+      <c r="Z20" s="193"/>
       <c r="AA20" s="193"/>
       <c r="AB20" s="193"/>
       <c r="AC20" s="193"/>
-      <c r="AD20" s="193"/>
-    </row>
-    <row r="21" spans="1:34" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="190"/>
       <c r="C21" s="190"/>
       <c r="D21" s="190"/>
       <c r="E21" s="190"/>
       <c r="F21" s="190"/>
-      <c r="G21" s="190"/>
-      <c r="H21" s="182"/>
+      <c r="G21" s="182"/>
+      <c r="H21" s="190"/>
       <c r="I21" s="190"/>
       <c r="J21" s="190"/>
-      <c r="K21" s="190"/>
+      <c r="K21" s="185"/>
       <c r="L21" s="185"/>
       <c r="M21" s="185"/>
       <c r="N21" s="185"/>
@@ -16845,39 +16810,38 @@
       <c r="P21" s="185"/>
       <c r="Q21" s="185"/>
       <c r="R21" s="185"/>
-      <c r="S21" s="185"/>
+      <c r="S21" s="194"/>
       <c r="T21" s="194"/>
       <c r="U21" s="194"/>
       <c r="V21" s="194"/>
       <c r="W21" s="194"/>
       <c r="X21" s="194"/>
       <c r="Y21" s="194"/>
-      <c r="Z21" s="194"/>
+      <c r="Z21" s="193"/>
       <c r="AA21" s="193"/>
       <c r="AB21" s="193"/>
       <c r="AC21" s="193"/>
-      <c r="AD21" s="193"/>
-    </row>
-    <row r="22" spans="1:34" s="181" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:33" s="181" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="189"/>
-      <c r="B22" s="309" t="s">
+      <c r="B22" s="280" t="s">
         <v>160</v>
       </c>
-      <c r="C22" s="305" t="s">
+      <c r="C22" s="294" t="s">
         <v>157</v>
       </c>
-      <c r="D22" s="306"/>
-      <c r="E22" s="294" t="s">
+      <c r="D22" s="317" t="s">
         <v>301</v>
       </c>
-      <c r="F22" s="295"/>
-      <c r="G22" s="295"/>
-      <c r="H22" s="295"/>
-      <c r="I22" s="295"/>
-      <c r="J22" s="296"/>
-      <c r="K22" s="303" t="s">
+      <c r="E22" s="318"/>
+      <c r="F22" s="318"/>
+      <c r="G22" s="318"/>
+      <c r="H22" s="318"/>
+      <c r="I22" s="319"/>
+      <c r="J22" s="292" t="s">
         <v>340</v>
       </c>
+      <c r="K22" s="197"/>
       <c r="L22" s="197"/>
       <c r="M22" s="197"/>
       <c r="N22" s="197"/>
@@ -16896,26 +16860,25 @@
       <c r="AA22" s="197"/>
       <c r="AB22" s="197"/>
       <c r="AC22" s="197"/>
-      <c r="AD22" s="197"/>
+      <c r="AD22" s="180"/>
       <c r="AE22" s="180"/>
       <c r="AF22" s="180"/>
       <c r="AG22" s="180"/>
-      <c r="AH22" s="180"/>
-    </row>
-    <row r="23" spans="1:34" s="181" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:33" s="181" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="189"/>
-      <c r="B23" s="310"/>
-      <c r="C23" s="307"/>
-      <c r="D23" s="308"/>
-      <c r="E23" s="297" t="s">
+      <c r="B23" s="281"/>
+      <c r="C23" s="295"/>
+      <c r="D23" s="320" t="s">
         <v>341</v>
       </c>
-      <c r="F23" s="298"/>
-      <c r="G23" s="298"/>
-      <c r="H23" s="298"/>
-      <c r="I23" s="298"/>
-      <c r="J23" s="298"/>
-      <c r="K23" s="304"/>
+      <c r="E23" s="321"/>
+      <c r="F23" s="321"/>
+      <c r="G23" s="321"/>
+      <c r="H23" s="321"/>
+      <c r="I23" s="321"/>
+      <c r="J23" s="293"/>
+      <c r="K23" s="198"/>
       <c r="L23" s="198"/>
       <c r="M23" s="198"/>
       <c r="N23" s="198"/>
@@ -16933,37 +16896,36 @@
       <c r="Z23" s="198"/>
       <c r="AA23" s="198"/>
       <c r="AB23" s="198"/>
-      <c r="AC23" s="198"/>
-      <c r="AD23" s="195"/>
+      <c r="AC23" s="195"/>
+      <c r="AD23" s="180"/>
       <c r="AE23" s="180"/>
       <c r="AF23" s="180"/>
       <c r="AG23" s="180"/>
-      <c r="AH23" s="180"/>
-    </row>
-    <row r="24" spans="1:34" s="181" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:33" s="181" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="189"/>
-      <c r="B24" s="310"/>
-      <c r="C24" s="307"/>
-      <c r="D24" s="308"/>
-      <c r="E24" s="292" t="s">
+      <c r="B24" s="281"/>
+      <c r="C24" s="295"/>
+      <c r="D24" s="284" t="s">
         <v>343</v>
       </c>
-      <c r="F24" s="292" t="s">
-        <v>368</v>
-      </c>
-      <c r="G24" s="290" t="s">
+      <c r="E24" s="284" t="s">
+        <v>367</v>
+      </c>
+      <c r="F24" s="315" t="s">
         <v>345</v>
       </c>
-      <c r="H24" s="313" t="s">
+      <c r="G24" s="286" t="s">
         <v>345</v>
       </c>
-      <c r="I24" s="313" t="s">
+      <c r="H24" s="286" t="s">
         <v>345</v>
       </c>
-      <c r="J24" s="292" t="s">
+      <c r="I24" s="284" t="s">
         <v>344</v>
       </c>
-      <c r="K24" s="304"/>
+      <c r="J24" s="293"/>
+      <c r="K24" s="189"/>
       <c r="L24" s="189"/>
       <c r="M24" s="189"/>
       <c r="N24" s="189"/>
@@ -16982,20 +16944,19 @@
       <c r="AA24" s="189"/>
       <c r="AB24" s="189"/>
       <c r="AC24" s="189"/>
-      <c r="AD24" s="189"/>
-    </row>
-    <row r="25" spans="1:34" s="181" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:33" s="181" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="189"/>
-      <c r="B25" s="310"/>
-      <c r="C25" s="307"/>
-      <c r="D25" s="308"/>
-      <c r="E25" s="292"/>
-      <c r="F25" s="292"/>
-      <c r="G25" s="291"/>
-      <c r="H25" s="313"/>
-      <c r="I25" s="313"/>
-      <c r="J25" s="292"/>
-      <c r="K25" s="304"/>
+      <c r="B25" s="281"/>
+      <c r="C25" s="295"/>
+      <c r="D25" s="284"/>
+      <c r="E25" s="284"/>
+      <c r="F25" s="316"/>
+      <c r="G25" s="286"/>
+      <c r="H25" s="286"/>
+      <c r="I25" s="284"/>
+      <c r="J25" s="293"/>
+      <c r="K25" s="189"/>
       <c r="L25" s="189"/>
       <c r="M25" s="189"/>
       <c r="N25" s="189"/>
@@ -17014,22 +16975,21 @@
       <c r="AA25" s="189"/>
       <c r="AB25" s="189"/>
       <c r="AC25" s="189"/>
-      <c r="AD25" s="189"/>
-    </row>
-    <row r="26" spans="1:34" s="181" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:33" s="181" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="189"/>
-      <c r="B26" s="311"/>
-      <c r="C26" s="307"/>
-      <c r="D26" s="308"/>
-      <c r="E26" s="293"/>
-      <c r="F26" s="293"/>
-      <c r="G26" s="218" t="s">
+      <c r="B26" s="282"/>
+      <c r="C26" s="295"/>
+      <c r="D26" s="285"/>
+      <c r="E26" s="285"/>
+      <c r="F26" s="218" t="s">
         <v>354</v>
       </c>
+      <c r="G26" s="219"/>
       <c r="H26" s="219"/>
-      <c r="I26" s="219"/>
+      <c r="I26" s="285"/>
       <c r="J26" s="293"/>
-      <c r="K26" s="304"/>
+      <c r="K26" s="189"/>
       <c r="L26" s="189"/>
       <c r="M26" s="189"/>
       <c r="N26" s="189"/>
@@ -17048,20 +17008,19 @@
       <c r="AA26" s="189"/>
       <c r="AB26" s="189"/>
       <c r="AC26" s="189"/>
-      <c r="AD26" s="189"/>
-    </row>
-    <row r="27" spans="1:34" s="181" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:33" s="181" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="189"/>
       <c r="B27" s="220"/>
-      <c r="C27" s="286"/>
-      <c r="D27" s="287"/>
-      <c r="E27" s="202"/>
-      <c r="F27" s="221"/>
-      <c r="G27" s="222"/>
+      <c r="C27" s="230"/>
+      <c r="D27" s="202"/>
+      <c r="E27" s="221"/>
+      <c r="F27" s="222"/>
+      <c r="G27" s="223"/>
       <c r="H27" s="223"/>
-      <c r="I27" s="223"/>
-      <c r="J27" s="224"/>
-      <c r="K27" s="225"/>
+      <c r="I27" s="224"/>
+      <c r="J27" s="225"/>
+      <c r="K27" s="189"/>
       <c r="L27" s="189"/>
       <c r="M27" s="189"/>
       <c r="N27" s="189"/>
@@ -17080,20 +17039,19 @@
       <c r="AA27" s="189"/>
       <c r="AB27" s="189"/>
       <c r="AC27" s="189"/>
-      <c r="AD27" s="189"/>
-    </row>
-    <row r="28" spans="1:34" s="181" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:33" s="181" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="189"/>
       <c r="B28" s="183"/>
-      <c r="C28" s="288"/>
-      <c r="D28" s="289"/>
-      <c r="E28" s="203"/>
+      <c r="C28" s="231"/>
+      <c r="D28" s="203"/>
+      <c r="E28" s="204"/>
       <c r="F28" s="204"/>
-      <c r="G28" s="204"/>
+      <c r="G28" s="184"/>
       <c r="H28" s="184"/>
-      <c r="I28" s="184"/>
-      <c r="J28" s="200"/>
-      <c r="K28" s="201"/>
+      <c r="I28" s="200"/>
+      <c r="J28" s="201"/>
+      <c r="K28" s="189"/>
       <c r="L28" s="189"/>
       <c r="M28" s="189"/>
       <c r="N28" s="189"/>
@@ -17112,19 +17070,18 @@
       <c r="AA28" s="189"/>
       <c r="AB28" s="189"/>
       <c r="AC28" s="189"/>
-      <c r="AD28" s="189"/>
-    </row>
-    <row r="29" spans="1:34" s="181" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:33" s="181" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="189"/>
       <c r="B29" s="211"/>
       <c r="C29" s="212"/>
-      <c r="D29" s="212"/>
-      <c r="E29" s="213"/>
+      <c r="D29" s="213"/>
+      <c r="E29" s="214"/>
       <c r="F29" s="214"/>
-      <c r="G29" s="214"/>
+      <c r="G29" s="215"/>
       <c r="H29" s="215"/>
       <c r="I29" s="215"/>
-      <c r="J29" s="215"/>
+      <c r="J29" s="189"/>
       <c r="K29" s="189"/>
       <c r="L29" s="189"/>
       <c r="M29" s="189"/>
@@ -17144,91 +17101,88 @@
       <c r="AA29" s="189"/>
       <c r="AB29" s="189"/>
       <c r="AC29" s="189"/>
-      <c r="AD29" s="189"/>
-    </row>
-    <row r="30" spans="1:34" s="181" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:33" s="181" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="189"/>
       <c r="B30" s="188"/>
-      <c r="C30" s="336" t="s">
+      <c r="C30" s="232" t="s">
         <v>348</v>
       </c>
-      <c r="D30" s="337"/>
-      <c r="E30" s="337"/>
-      <c r="F30" s="337"/>
-      <c r="G30" s="337"/>
-      <c r="H30" s="337"/>
-      <c r="I30" s="267"/>
-      <c r="J30" s="268"/>
-      <c r="K30" s="314"/>
-      <c r="L30" s="314"/>
-      <c r="M30" s="314"/>
+      <c r="D30" s="233"/>
+      <c r="E30" s="233"/>
+      <c r="F30" s="233"/>
+      <c r="G30" s="233"/>
+      <c r="H30" s="287"/>
+      <c r="I30" s="288"/>
+      <c r="J30" s="289"/>
+      <c r="K30" s="289"/>
+      <c r="L30" s="289"/>
+      <c r="M30" s="187"/>
       <c r="N30" s="187"/>
       <c r="O30" s="187"/>
-      <c r="P30" s="187"/>
-      <c r="Q30" s="199"/>
+      <c r="P30" s="199"/>
+      <c r="Q30" s="187"/>
       <c r="R30" s="187"/>
       <c r="S30" s="187"/>
       <c r="T30" s="187"/>
       <c r="U30" s="187"/>
-      <c r="V30" s="187"/>
-      <c r="W30" s="315"/>
-      <c r="X30" s="315"/>
-      <c r="Y30" s="314"/>
-      <c r="Z30" s="314"/>
-      <c r="AA30" s="314"/>
-      <c r="AB30" s="314"/>
-      <c r="AC30" s="314"/>
-      <c r="AD30" s="185"/>
-    </row>
-    <row r="31" spans="1:34" s="181" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V30" s="290"/>
+      <c r="W30" s="290"/>
+      <c r="X30" s="289"/>
+      <c r="Y30" s="289"/>
+      <c r="Z30" s="289"/>
+      <c r="AA30" s="289"/>
+      <c r="AB30" s="289"/>
+      <c r="AC30" s="185"/>
+    </row>
+    <row r="31" spans="1:33" s="181" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="189"/>
       <c r="B31" s="188"/>
-      <c r="C31" s="338" t="s">
+      <c r="C31" s="234" t="s">
         <v>351</v>
       </c>
-      <c r="D31" s="339"/>
-      <c r="E31" s="339"/>
-      <c r="F31" s="339"/>
-      <c r="G31" s="339"/>
-      <c r="H31" s="339"/>
-      <c r="I31" s="267"/>
-      <c r="J31" s="268"/>
-      <c r="K31" s="185"/>
+      <c r="D31" s="235"/>
+      <c r="E31" s="235"/>
+      <c r="F31" s="235"/>
+      <c r="G31" s="235"/>
+      <c r="H31" s="287"/>
+      <c r="I31" s="288"/>
+      <c r="J31" s="185"/>
+      <c r="K31" s="189"/>
       <c r="L31" s="189"/>
       <c r="M31" s="189"/>
       <c r="N31" s="189"/>
-      <c r="O31" s="189"/>
+      <c r="O31" s="187"/>
       <c r="P31" s="187"/>
       <c r="Q31" s="187"/>
       <c r="R31" s="187"/>
       <c r="S31" s="187"/>
       <c r="T31" s="187"/>
       <c r="U31" s="187"/>
-      <c r="V31" s="187"/>
+      <c r="V31" s="186"/>
       <c r="W31" s="186"/>
-      <c r="X31" s="186"/>
+      <c r="X31" s="185"/>
       <c r="Y31" s="185"/>
       <c r="Z31" s="185"/>
       <c r="AA31" s="185"/>
       <c r="AB31" s="185"/>
       <c r="AC31" s="185"/>
-      <c r="AD31" s="185"/>
-    </row>
-    <row r="32" spans="1:34" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:33" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="188"/>
-      <c r="C32" s="340" t="s">
+      <c r="C32" s="236" t="s">
         <v>347</v>
       </c>
-      <c r="D32" s="341"/>
-      <c r="E32" s="341"/>
-      <c r="F32" s="341"/>
-      <c r="G32" s="341"/>
-      <c r="H32" s="341"/>
-      <c r="I32" s="267"/>
-      <c r="J32" s="268"/>
-      <c r="K32" s="314"/>
-      <c r="L32" s="314"/>
-      <c r="M32" s="314"/>
+      <c r="D32" s="237"/>
+      <c r="E32" s="237"/>
+      <c r="F32" s="237"/>
+      <c r="G32" s="237"/>
+      <c r="H32" s="287"/>
+      <c r="I32" s="288"/>
+      <c r="J32" s="289"/>
+      <c r="K32" s="289"/>
+      <c r="L32" s="289"/>
+      <c r="M32" s="187"/>
       <c r="N32" s="187"/>
       <c r="O32" s="187"/>
       <c r="P32" s="187"/>
@@ -17238,27 +17192,26 @@
       <c r="T32" s="187"/>
       <c r="U32" s="187"/>
       <c r="V32" s="187"/>
-      <c r="W32" s="187"/>
-      <c r="X32" s="316"/>
-      <c r="Y32" s="316"/>
-      <c r="Z32" s="316"/>
+      <c r="W32" s="291"/>
+      <c r="X32" s="291"/>
+      <c r="Y32" s="291"/>
+      <c r="Z32" s="187"/>
       <c r="AA32" s="187"/>
       <c r="AB32" s="187"/>
       <c r="AC32" s="187"/>
-      <c r="AD32" s="187"/>
-    </row>
-    <row r="33" spans="2:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="188"/>
-      <c r="C33" s="340" t="s">
+      <c r="C33" s="236" t="s">
         <v>349</v>
       </c>
-      <c r="D33" s="341"/>
-      <c r="E33" s="341"/>
-      <c r="F33" s="341"/>
-      <c r="G33" s="341"/>
-      <c r="H33" s="341"/>
-      <c r="I33" s="267"/>
-      <c r="J33" s="268"/>
+      <c r="D33" s="237"/>
+      <c r="E33" s="237"/>
+      <c r="F33" s="237"/>
+      <c r="G33" s="237"/>
+      <c r="H33" s="287"/>
+      <c r="I33" s="288"/>
+      <c r="J33" s="187"/>
       <c r="K33" s="187"/>
       <c r="L33" s="187"/>
       <c r="M33" s="187"/>
@@ -17271,27 +17224,26 @@
       <c r="T33" s="187"/>
       <c r="U33" s="187"/>
       <c r="V33" s="187"/>
-      <c r="W33" s="187"/>
-      <c r="X33" s="312"/>
-      <c r="Y33" s="312"/>
-      <c r="Z33" s="312"/>
-      <c r="AA33" s="312"/>
-      <c r="AB33" s="312"/>
+      <c r="W33" s="283"/>
+      <c r="X33" s="283"/>
+      <c r="Y33" s="283"/>
+      <c r="Z33" s="283"/>
+      <c r="AA33" s="283"/>
+      <c r="AB33" s="187"/>
       <c r="AC33" s="187"/>
-      <c r="AD33" s="187"/>
-    </row>
-    <row r="34" spans="2:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="188"/>
-      <c r="C34" s="338" t="s">
+      <c r="C34" s="234" t="s">
         <v>350</v>
       </c>
-      <c r="D34" s="339"/>
-      <c r="E34" s="339"/>
-      <c r="F34" s="339"/>
-      <c r="G34" s="339"/>
-      <c r="H34" s="339"/>
-      <c r="I34" s="267"/>
-      <c r="J34" s="268"/>
+      <c r="D34" s="235"/>
+      <c r="E34" s="235"/>
+      <c r="F34" s="235"/>
+      <c r="G34" s="235"/>
+      <c r="H34" s="287"/>
+      <c r="I34" s="288"/>
+      <c r="J34" s="187"/>
       <c r="K34" s="187"/>
       <c r="L34" s="187"/>
       <c r="M34" s="187"/>
@@ -17311,21 +17263,20 @@
       <c r="AA34" s="187"/>
       <c r="AB34" s="187"/>
       <c r="AC34" s="187"/>
-      <c r="AD34" s="187"/>
-    </row>
-    <row r="35" spans="2:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="190"/>
-      <c r="C35" s="342" t="s">
+      <c r="C35" s="238" t="s">
         <v>352</v>
       </c>
-      <c r="D35" s="343"/>
-      <c r="E35" s="343"/>
-      <c r="F35" s="343"/>
-      <c r="G35" s="343"/>
-      <c r="H35" s="343"/>
-      <c r="I35" s="267"/>
-      <c r="J35" s="268"/>
-      <c r="K35" s="191"/>
+      <c r="D35" s="239"/>
+      <c r="E35" s="239"/>
+      <c r="F35" s="239"/>
+      <c r="G35" s="239"/>
+      <c r="H35" s="287"/>
+      <c r="I35" s="288"/>
+      <c r="J35" s="191"/>
+      <c r="K35" s="190"/>
       <c r="L35" s="190"/>
       <c r="M35" s="190"/>
       <c r="N35" s="190"/>
@@ -17337,16 +17288,15 @@
       <c r="T35" s="190"/>
       <c r="U35" s="190"/>
       <c r="V35" s="190"/>
-      <c r="W35" s="190"/>
-      <c r="X35" s="192"/>
+      <c r="W35" s="192"/>
+      <c r="X35" s="190"/>
       <c r="Y35" s="190"/>
       <c r="Z35" s="190"/>
       <c r="AA35" s="190"/>
       <c r="AB35" s="190"/>
       <c r="AC35" s="190"/>
-      <c r="AD35" s="190"/>
-    </row>
-    <row r="36" spans="2:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B36" s="190"/>
       <c r="C36" s="190"/>
       <c r="D36" s="190"/>
@@ -17375,62 +17325,50 @@
       <c r="AA36" s="190"/>
       <c r="AB36" s="190"/>
       <c r="AC36" s="190"/>
-      <c r="AD36" s="190"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
+  <mergeCells count="38">
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="D22:I22"/>
+    <mergeCell ref="D23:I23"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="D10:I10"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="D12:I12"/>
+    <mergeCell ref="C1:I2"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D7:I7"/>
     <mergeCell ref="B22:B26"/>
-    <mergeCell ref="X33:AB33"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="W33:AA33"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="G24:G25"/>
     <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K32:M32"/>
-    <mergeCell ref="W30:X30"/>
-    <mergeCell ref="Y30:AC30"/>
-    <mergeCell ref="X32:Z32"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="K22:K26"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C22:D26"/>
-    <mergeCell ref="D12:J12"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="C1:J2"/>
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="C19:I19"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="X30:AB30"/>
+    <mergeCell ref="W32:Y32"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="J22:J26"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H31:I31"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="Q30">
+  <conditionalFormatting sqref="P30">
     <cfRule type="cellIs" dxfId="1" priority="728" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -17440,7 +17378,7 @@
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="85" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17468,72 +17406,72 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="318" t="s">
+      <c r="B2" s="323" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="319"/>
-      <c r="D2" s="319"/>
-      <c r="E2" s="319"/>
-      <c r="F2" s="319"/>
-      <c r="G2" s="319"/>
-      <c r="H2" s="319"/>
-      <c r="I2" s="319"/>
-      <c r="J2" s="319"/>
-      <c r="K2" s="319"/>
-      <c r="L2" s="319"/>
-      <c r="M2" s="320"/>
+      <c r="C2" s="324"/>
+      <c r="D2" s="324"/>
+      <c r="E2" s="324"/>
+      <c r="F2" s="324"/>
+      <c r="G2" s="324"/>
+      <c r="H2" s="324"/>
+      <c r="I2" s="324"/>
+      <c r="J2" s="324"/>
+      <c r="K2" s="324"/>
+      <c r="L2" s="324"/>
+      <c r="M2" s="325"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="321" t="s">
+      <c r="B3" s="326" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="323" t="s">
+      <c r="C3" s="328" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="323" t="s">
+      <c r="D3" s="328" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="325" t="s">
+      <c r="E3" s="330" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="327" t="s">
+      <c r="F3" s="332" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="328"/>
-      <c r="H3" s="328"/>
-      <c r="I3" s="328"/>
-      <c r="J3" s="328"/>
-      <c r="K3" s="328"/>
-      <c r="L3" s="328"/>
-      <c r="M3" s="329"/>
+      <c r="G3" s="333"/>
+      <c r="H3" s="333"/>
+      <c r="I3" s="333"/>
+      <c r="J3" s="333"/>
+      <c r="K3" s="333"/>
+      <c r="L3" s="333"/>
+      <c r="M3" s="334"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="322"/>
-      <c r="C4" s="324"/>
-      <c r="D4" s="324"/>
-      <c r="E4" s="326"/>
-      <c r="F4" s="330"/>
-      <c r="G4" s="331"/>
-      <c r="H4" s="331"/>
-      <c r="I4" s="331"/>
-      <c r="J4" s="331"/>
-      <c r="K4" s="331"/>
-      <c r="L4" s="331"/>
-      <c r="M4" s="332"/>
+      <c r="B4" s="327"/>
+      <c r="C4" s="329"/>
+      <c r="D4" s="329"/>
+      <c r="E4" s="331"/>
+      <c r="F4" s="335"/>
+      <c r="G4" s="336"/>
+      <c r="H4" s="336"/>
+      <c r="I4" s="336"/>
+      <c r="J4" s="336"/>
+      <c r="K4" s="336"/>
+      <c r="L4" s="336"/>
+      <c r="M4" s="337"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="317"/>
-      <c r="C5" s="317"/>
-      <c r="D5" s="317"/>
-      <c r="E5" s="317"/>
-      <c r="F5" s="317"/>
-      <c r="G5" s="317"/>
-      <c r="H5" s="317"/>
-      <c r="I5" s="317"/>
-      <c r="J5" s="317"/>
-      <c r="K5" s="317"/>
-      <c r="L5" s="317"/>
-      <c r="M5" s="317"/>
+      <c r="B5" s="322"/>
+      <c r="C5" s="322"/>
+      <c r="D5" s="322"/>
+      <c r="E5" s="322"/>
+      <c r="F5" s="322"/>
+      <c r="G5" s="322"/>
+      <c r="H5" s="322"/>
+      <c r="I5" s="322"/>
+      <c r="J5" s="322"/>
+      <c r="K5" s="322"/>
+      <c r="L5" s="322"/>
+      <c r="M5" s="322"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -18146,72 +18084,72 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="318" t="s">
+      <c r="B2" s="323" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="319"/>
-      <c r="D2" s="319"/>
-      <c r="E2" s="319"/>
-      <c r="F2" s="319"/>
-      <c r="G2" s="319"/>
-      <c r="H2" s="319"/>
-      <c r="I2" s="319"/>
-      <c r="J2" s="319"/>
-      <c r="K2" s="319"/>
-      <c r="L2" s="319"/>
-      <c r="M2" s="320"/>
+      <c r="C2" s="324"/>
+      <c r="D2" s="324"/>
+      <c r="E2" s="324"/>
+      <c r="F2" s="324"/>
+      <c r="G2" s="324"/>
+      <c r="H2" s="324"/>
+      <c r="I2" s="324"/>
+      <c r="J2" s="324"/>
+      <c r="K2" s="324"/>
+      <c r="L2" s="324"/>
+      <c r="M2" s="325"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="321" t="s">
+      <c r="B3" s="326" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="323" t="s">
+      <c r="C3" s="328" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="323" t="s">
+      <c r="D3" s="328" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="325" t="s">
+      <c r="E3" s="330" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="327" t="s">
+      <c r="F3" s="332" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="328"/>
-      <c r="H3" s="328"/>
-      <c r="I3" s="328"/>
-      <c r="J3" s="328"/>
-      <c r="K3" s="328"/>
-      <c r="L3" s="328"/>
-      <c r="M3" s="329"/>
+      <c r="G3" s="333"/>
+      <c r="H3" s="333"/>
+      <c r="I3" s="333"/>
+      <c r="J3" s="333"/>
+      <c r="K3" s="333"/>
+      <c r="L3" s="333"/>
+      <c r="M3" s="334"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="322"/>
-      <c r="C4" s="324"/>
-      <c r="D4" s="324"/>
-      <c r="E4" s="326"/>
-      <c r="F4" s="330"/>
-      <c r="G4" s="331"/>
-      <c r="H4" s="331"/>
-      <c r="I4" s="331"/>
-      <c r="J4" s="331"/>
-      <c r="K4" s="331"/>
-      <c r="L4" s="331"/>
-      <c r="M4" s="332"/>
+      <c r="B4" s="327"/>
+      <c r="C4" s="329"/>
+      <c r="D4" s="329"/>
+      <c r="E4" s="331"/>
+      <c r="F4" s="335"/>
+      <c r="G4" s="336"/>
+      <c r="H4" s="336"/>
+      <c r="I4" s="336"/>
+      <c r="J4" s="336"/>
+      <c r="K4" s="336"/>
+      <c r="L4" s="336"/>
+      <c r="M4" s="337"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="317"/>
-      <c r="C5" s="317"/>
-      <c r="D5" s="317"/>
-      <c r="E5" s="317"/>
-      <c r="F5" s="333"/>
-      <c r="G5" s="333"/>
-      <c r="H5" s="333"/>
-      <c r="I5" s="333"/>
-      <c r="J5" s="333"/>
-      <c r="K5" s="333"/>
-      <c r="L5" s="333"/>
-      <c r="M5" s="333"/>
+      <c r="B5" s="322"/>
+      <c r="C5" s="322"/>
+      <c r="D5" s="322"/>
+      <c r="E5" s="322"/>
+      <c r="F5" s="338"/>
+      <c r="G5" s="338"/>
+      <c r="H5" s="338"/>
+      <c r="I5" s="338"/>
+      <c r="J5" s="338"/>
+      <c r="K5" s="338"/>
+      <c r="L5" s="338"/>
+      <c r="M5" s="338"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -18812,72 +18750,72 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="318" t="s">
+      <c r="B2" s="323" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="319"/>
-      <c r="D2" s="319"/>
-      <c r="E2" s="319"/>
-      <c r="F2" s="319"/>
-      <c r="G2" s="319"/>
-      <c r="H2" s="319"/>
-      <c r="I2" s="319"/>
-      <c r="J2" s="319"/>
-      <c r="K2" s="319"/>
-      <c r="L2" s="319"/>
-      <c r="M2" s="320"/>
+      <c r="C2" s="324"/>
+      <c r="D2" s="324"/>
+      <c r="E2" s="324"/>
+      <c r="F2" s="324"/>
+      <c r="G2" s="324"/>
+      <c r="H2" s="324"/>
+      <c r="I2" s="324"/>
+      <c r="J2" s="324"/>
+      <c r="K2" s="324"/>
+      <c r="L2" s="324"/>
+      <c r="M2" s="325"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="321" t="s">
+      <c r="B3" s="326" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="323" t="s">
+      <c r="C3" s="328" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="323" t="s">
+      <c r="D3" s="328" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="325" t="s">
+      <c r="E3" s="330" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="327" t="s">
+      <c r="F3" s="332" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="328"/>
-      <c r="H3" s="328"/>
-      <c r="I3" s="328"/>
-      <c r="J3" s="328"/>
-      <c r="K3" s="328"/>
-      <c r="L3" s="328"/>
-      <c r="M3" s="329"/>
+      <c r="G3" s="333"/>
+      <c r="H3" s="333"/>
+      <c r="I3" s="333"/>
+      <c r="J3" s="333"/>
+      <c r="K3" s="333"/>
+      <c r="L3" s="333"/>
+      <c r="M3" s="334"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="322"/>
-      <c r="C4" s="324"/>
-      <c r="D4" s="324"/>
-      <c r="E4" s="326"/>
-      <c r="F4" s="330"/>
-      <c r="G4" s="331"/>
-      <c r="H4" s="331"/>
-      <c r="I4" s="331"/>
-      <c r="J4" s="331"/>
-      <c r="K4" s="331"/>
-      <c r="L4" s="331"/>
-      <c r="M4" s="332"/>
+      <c r="B4" s="327"/>
+      <c r="C4" s="329"/>
+      <c r="D4" s="329"/>
+      <c r="E4" s="331"/>
+      <c r="F4" s="335"/>
+      <c r="G4" s="336"/>
+      <c r="H4" s="336"/>
+      <c r="I4" s="336"/>
+      <c r="J4" s="336"/>
+      <c r="K4" s="336"/>
+      <c r="L4" s="336"/>
+      <c r="M4" s="337"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="334"/>
-      <c r="C5" s="317"/>
-      <c r="D5" s="317"/>
-      <c r="E5" s="317"/>
-      <c r="F5" s="317"/>
-      <c r="G5" s="317"/>
-      <c r="H5" s="317"/>
-      <c r="I5" s="317"/>
-      <c r="J5" s="317"/>
-      <c r="K5" s="317"/>
-      <c r="L5" s="317"/>
-      <c r="M5" s="335"/>
+      <c r="B5" s="339"/>
+      <c r="C5" s="322"/>
+      <c r="D5" s="322"/>
+      <c r="E5" s="322"/>
+      <c r="F5" s="322"/>
+      <c r="G5" s="322"/>
+      <c r="H5" s="322"/>
+      <c r="I5" s="322"/>
+      <c r="J5" s="322"/>
+      <c r="K5" s="322"/>
+      <c r="L5" s="322"/>
+      <c r="M5" s="340"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">

</xml_diff>